<commit_message>
consistent naming for searches
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE169FB-7E8D-4AE2-BCE4-BCE6FB713F06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A334B3-22EF-49E5-96B6-179EB96F4AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,30 +108,8 @@
 </connections>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="459">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1351,39 +1329,9 @@
     <t>DatasetRecordClasses.DatasetRecordClass.Searches</t>
   </si>
   <si>
-    <t>GeneQuestions.upload</t>
-  </si>
-  <si>
-    <t>GeneQuestions.id</t>
-  </si>
-  <si>
-    <t>GeneQuestions.keyword</t>
-  </si>
-  <si>
-    <t>GeneDataset.proteomics_comparison</t>
-  </si>
-  <si>
-    <t>Study001.study001_comparison</t>
-  </si>
-  <si>
-    <t>Study001.study001_expression</t>
-  </si>
-  <si>
-    <t>Study002.study002_comparison</t>
-  </si>
-  <si>
-    <t>Study002.study002_expression</t>
-  </si>
-  <si>
-    <t>Study005.study005_comparison</t>
-  </si>
-  <si>
     <t>Study005.study005_expression</t>
   </si>
   <si>
-    <t>GeneQuestions.go</t>
-  </si>
-  <si>
     <t>## Mouse Gene Attributes ##</t>
   </si>
   <si>
@@ -1496,6 +1444,48 @@
   </si>
   <si>
     <t>study003_comparisons</t>
+  </si>
+  <si>
+    <t>MouseGeneQuestions.go</t>
+  </si>
+  <si>
+    <t>HumanGeneQuestions.go</t>
+  </si>
+  <si>
+    <t>MouseGeneQuestions.upload</t>
+  </si>
+  <si>
+    <t>HumanGeneQuestions.upload</t>
+  </si>
+  <si>
+    <t>MouseGeneQuestions.pathways</t>
+  </si>
+  <si>
+    <t>HumanGeneQuestions.pathways</t>
+  </si>
+  <si>
+    <t>study003_questions.study003_comparison</t>
+  </si>
+  <si>
+    <t>Attributes ##</t>
+  </si>
+  <si>
+    <t>study001_questions.study001_comparison</t>
+  </si>
+  <si>
+    <t>study001_questions.study001_expression</t>
+  </si>
+  <si>
+    <t>study002_questions.study002_comparison</t>
+  </si>
+  <si>
+    <t>study002_questions.study002_expression</t>
+  </si>
+  <si>
+    <t>study005_questions.study005_comparison</t>
+  </si>
+  <si>
+    <t>study005_questions.study005_expression</t>
   </si>
 </sst>
 </file>
@@ -1826,21 +1816,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N167"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C68" sqref="C68"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="80.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.625" bestFit="1" customWidth="1"/>
@@ -1965,7 +1955,7 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE(D10,".",F10)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.GeneQuestions.keyword</v>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.HumanGeneQuestions.upload</v>
       </c>
       <c r="B10" t="s">
         <v>155</v>
@@ -1974,25 +1964,22 @@
         <v>156</v>
       </c>
       <c r="D10" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>408</v>
+        <v>448</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
       </c>
-      <c r="M10" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" ref="A11:A20" si="0">CONCATENATE(D11,".",F11)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.GeneQuestions.id</v>
+        <f t="shared" ref="A11:A22" si="0">CONCATENATE(D11,".",F11)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.MouseGeneQuestions.upload</v>
       </c>
       <c r="B11" t="s">
         <v>155</v>
@@ -2001,25 +1988,22 @@
         <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>407</v>
+        <v>447</v>
       </c>
       <c r="L11" t="s">
         <v>27</v>
-      </c>
-      <c r="M11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.GeneQuestions.upload</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.MouseGeneQuestions.go</v>
       </c>
       <c r="B12" t="s">
         <v>155</v>
@@ -2028,13 +2012,13 @@
         <v>156</v>
       </c>
       <c r="D12" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
       <c r="L12" t="s">
         <v>27</v>
@@ -2042,8 +2026,8 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.GeneQuestions.go</v>
+        <f t="shared" ref="A13:A14" si="1">CONCATENATE(D13,".",F13)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.HumanGeneQuestions.go</v>
       </c>
       <c r="B13" t="s">
         <v>155</v>
@@ -2052,13 +2036,13 @@
         <v>156</v>
       </c>
       <c r="D13" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>416</v>
+        <v>446</v>
       </c>
       <c r="L13" t="s">
         <v>27</v>
@@ -2066,23 +2050,23 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.GeneDataset.proteomics_comparison</v>
+        <f t="shared" si="1"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.MouseGeneQuestions.pathways</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>409</v>
+        <v>449</v>
       </c>
       <c r="L14" t="s">
         <v>27</v>
@@ -2090,26 +2074,23 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.Study001.study001_comparison</v>
+        <f t="shared" ref="A15" si="2">CONCATENATE(D15,".",F15)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.HumanGeneQuestions.pathways</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="D15" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>410</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
+        <v>450</v>
       </c>
       <c r="L15" t="s">
         <v>27</v>
@@ -2117,26 +2098,23 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.Study001.study001_expression</v>
-      </c>
-      <c r="B16" t="s">
-        <v>168</v>
+        <f>CONCATENATE(D16,".",F16)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_questions.study003_comparison</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>431</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>436</v>
       </c>
       <c r="D16" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>411</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
+        <v>451</v>
       </c>
       <c r="L16" t="s">
         <v>27</v>
@@ -2145,25 +2123,25 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.Study002.study002_comparison</v>
-      </c>
-      <c r="B17" t="s">
-        <v>168</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_comparison</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>429</v>
       </c>
       <c r="C17" t="s">
-        <v>169</v>
+        <v>433</v>
       </c>
       <c r="D17" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>412</v>
+        <v>453</v>
       </c>
       <c r="K17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L17" t="s">
         <v>27</v>
@@ -2172,25 +2150,25 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.Study002.study002_expression</v>
-      </c>
-      <c r="B18" t="s">
-        <v>168</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_expression</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>429</v>
       </c>
       <c r="C18" t="s">
-        <v>169</v>
+        <v>433</v>
       </c>
       <c r="D18" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>413</v>
+        <v>454</v>
       </c>
       <c r="K18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L18" t="s">
         <v>27</v>
@@ -2199,25 +2177,25 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.Study005.study005_comparison</v>
-      </c>
-      <c r="B19" t="s">
-        <v>168</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_comparison</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>430</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>432</v>
       </c>
       <c r="D19" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>414</v>
+        <v>455</v>
       </c>
       <c r="K19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L19" t="s">
         <v>27</v>
@@ -2226,105 +2204,93 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.Study005.study005_expression</v>
-      </c>
-      <c r="B20" t="s">
-        <v>168</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_expression</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>430</v>
       </c>
       <c r="C20" t="s">
-        <v>169</v>
+        <v>432</v>
       </c>
       <c r="D20" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>415</v>
+        <v>456</v>
       </c>
       <c r="K20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L20" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_comparison</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C21" t="s">
+        <v>437</v>
+      </c>
+      <c r="D21" t="s">
+        <v>420</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>457</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>417</v>
+      <c r="A22" t="str">
+        <f>CONCATENATE(D22,".",F22)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_expression</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C22" t="s">
+        <v>437</v>
+      </c>
+      <c r="D22" t="s">
+        <v>420</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>458</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="L22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f>CONCATENATE(D24,".",F24)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.source_id</v>
-      </c>
-      <c r="B24" t="s">
-        <v>155</v>
-      </c>
-      <c r="C24" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" t="s">
-        <v>430</v>
-      </c>
-      <c r="E24" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" t="s">
-        <v>127</v>
-      </c>
-      <c r="J24" t="s">
-        <v>193</v>
-      </c>
-      <c r="M24" t="s">
-        <v>197</v>
-      </c>
-      <c r="N24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <f t="shared" ref="A25:A47" si="1">CONCATENATE(D25,".",F25)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.organism</v>
-      </c>
-      <c r="B25" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" t="s">
-        <v>430</v>
-      </c>
-      <c r="E25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" t="s">
-        <v>396</v>
-      </c>
-      <c r="J25" t="s">
-        <v>193</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25" t="s">
-        <v>66</v>
-      </c>
-      <c r="M25" t="s">
-        <v>197</v>
-      </c>
-      <c r="N25" t="s">
-        <v>65</v>
+      <c r="A24" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>CONCATENATE(D26,".",F26)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.symbol</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.source_id</v>
       </c>
       <c r="B26" t="s">
         <v>155</v>
@@ -2333,23 +2299,17 @@
         <v>156</v>
       </c>
       <c r="D26" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E26" t="s">
         <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>243</v>
+        <v>127</v>
       </c>
       <c r="J26" t="s">
         <v>193</v>
       </c>
-      <c r="K26">
-        <v>2</v>
-      </c>
-      <c r="L26" t="s">
-        <v>66</v>
-      </c>
       <c r="M26" t="s">
         <v>197</v>
       </c>
@@ -2359,8 +2319,8 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.product</v>
+        <f t="shared" ref="A27:A49" si="3">CONCATENATE(D27,".",F27)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.organism</v>
       </c>
       <c r="B27" t="s">
         <v>155</v>
@@ -2369,19 +2329,19 @@
         <v>156</v>
       </c>
       <c r="D27" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E27" t="s">
         <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>396</v>
       </c>
       <c r="J27" t="s">
         <v>193</v>
       </c>
       <c r="K27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L27" t="s">
         <v>66</v>
@@ -2396,7 +2356,7 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>CONCATENATE(D28,".",F28)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.synonym</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.symbol</v>
       </c>
       <c r="B28" t="s">
         <v>155</v>
@@ -2405,19 +2365,19 @@
         <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E28" t="s">
         <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J28" t="s">
         <v>193</v>
       </c>
       <c r="K28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L28" t="s">
         <v>66</v>
@@ -2431,8 +2391,8 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.gene_type</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.product</v>
       </c>
       <c r="B29" t="s">
         <v>155</v>
@@ -2441,19 +2401,19 @@
         <v>156</v>
       </c>
       <c r="D29" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E29" t="s">
         <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>131</v>
       </c>
       <c r="J29" t="s">
         <v>193</v>
       </c>
       <c r="K29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L29" t="s">
         <v>66</v>
@@ -2468,7 +2428,7 @@
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>CONCATENATE(D30,".",F30)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_record_link</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.synonym</v>
       </c>
       <c r="B30" t="s">
         <v>155</v>
@@ -2477,19 +2437,19 @@
         <v>156</v>
       </c>
       <c r="D30" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E30" t="s">
         <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="J30" t="s">
         <v>193</v>
       </c>
       <c r="K30">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L30" t="s">
         <v>66</v>
@@ -2497,11 +2457,14 @@
       <c r="M30" t="s">
         <v>197</v>
       </c>
+      <c r="N30" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" ref="A31:A32" si="2">CONCATENATE(D31,".",F31)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_source_id</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.gene_type</v>
       </c>
       <c r="B31" t="s">
         <v>155</v>
@@ -2510,19 +2473,25 @@
         <v>156</v>
       </c>
       <c r="D31" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E31" t="s">
         <v>62</v>
       </c>
       <c r="F31" t="s">
-        <v>434</v>
+        <v>209</v>
       </c>
       <c r="J31" t="s">
         <v>193</v>
       </c>
       <c r="K31">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="L31" t="s">
+        <v>66</v>
+      </c>
+      <c r="M31" t="s">
+        <v>197</v>
       </c>
       <c r="N31" t="s">
         <v>65</v>
@@ -2530,8 +2499,8 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="2"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_symbol</v>
+        <f>CONCATENATE(D32,".",F32)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_record_link</v>
       </c>
       <c r="B32" t="s">
         <v>155</v>
@@ -2540,13 +2509,13 @@
         <v>156</v>
       </c>
       <c r="D32" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E32" t="s">
         <v>62</v>
       </c>
       <c r="F32" t="s">
-        <v>435</v>
+        <v>242</v>
       </c>
       <c r="J32" t="s">
         <v>193</v>
@@ -2554,41 +2523,38 @@
       <c r="K32">
         <v>6</v>
       </c>
-      <c r="N32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>CONCATENATE(D33,".",F33)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.locus</v>
+        <f t="shared" ref="A33:A34" si="4">CONCATENATE(D33,".",F33)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_source_id</v>
       </c>
       <c r="B33" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D33" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E33" t="s">
         <v>62</v>
       </c>
       <c r="F33" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="J33" t="s">
         <v>193</v>
       </c>
       <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33" t="s">
-        <v>66</v>
-      </c>
-      <c r="M33" t="s">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="N33" t="s">
         <v>65</v>
@@ -2596,44 +2562,38 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>CONCATENATE(D34,".",F34)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.location</v>
+        <f t="shared" si="4"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_symbol</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C34" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D34" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E34" t="s">
         <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="J34" t="s">
         <v>193</v>
       </c>
       <c r="K34">
-        <v>2</v>
-      </c>
-      <c r="L34" t="s">
-        <v>66</v>
-      </c>
-      <c r="M34" t="s">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="N34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>CONCATENATE(D35,".",F35)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.chromosome</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.locus</v>
       </c>
       <c r="B35" t="s">
         <v>162</v>
@@ -2642,17 +2602,20 @@
         <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E35" t="s">
         <v>62</v>
       </c>
       <c r="F35" t="s">
-        <v>208</v>
+        <v>422</v>
       </c>
       <c r="J35" t="s">
         <v>193</v>
       </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
       <c r="L35" t="s">
         <v>66</v>
       </c>
@@ -2665,8 +2628,8 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.strand</v>
+        <f>CONCATENATE(D36,".",F36)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.location</v>
       </c>
       <c r="B36" t="s">
         <v>162</v>
@@ -2675,17 +2638,20 @@
         <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E36" t="s">
         <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="J36" t="s">
         <v>193</v>
       </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
       <c r="L36" t="s">
         <v>66</v>
       </c>
@@ -2698,23 +2664,23 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.start_min</v>
+        <f>CONCATENATE(D37,".",F37)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.chromosome</v>
       </c>
       <c r="B37" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C37" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E37" t="s">
         <v>62</v>
       </c>
       <c r="F37" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="J37" t="s">
         <v>193</v>
@@ -2731,23 +2697,23 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.end_max</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.strand</v>
       </c>
       <c r="B38" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C38" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E38" t="s">
         <v>62</v>
       </c>
       <c r="F38" t="s">
-        <v>207</v>
+        <v>421</v>
       </c>
       <c r="J38" t="s">
         <v>193</v>
@@ -2764,29 +2730,32 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.gene_link_outs</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.start_min</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="C39" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="D39" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="F39" t="s">
-        <v>419</v>
+        <v>206</v>
       </c>
       <c r="J39" t="s">
         <v>193</v>
       </c>
+      <c r="L39" t="s">
+        <v>66</v>
+      </c>
       <c r="M39" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="N39" t="s">
         <v>65</v>
@@ -2794,29 +2763,32 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.protein_link_outs</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.end_max</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="D40" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E40" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="F40" t="s">
-        <v>420</v>
+        <v>207</v>
       </c>
       <c r="J40" t="s">
         <v>193</v>
       </c>
+      <c r="L40" t="s">
+        <v>66</v>
+      </c>
       <c r="M40" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="N40" t="s">
         <v>65</v>
@@ -2824,8 +2796,8 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.clinical_link_outs</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.gene_link_outs</v>
       </c>
       <c r="B41" t="s">
         <v>157</v>
@@ -2834,13 +2806,13 @@
         <v>159</v>
       </c>
       <c r="D41" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E41" t="s">
         <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="J41" t="s">
         <v>193</v>
@@ -2854,8 +2826,8 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.sequence_link_outs</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.protein_link_outs</v>
       </c>
       <c r="B42" t="s">
         <v>157</v>
@@ -2864,13 +2836,13 @@
         <v>159</v>
       </c>
       <c r="D42" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E42" t="s">
         <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="J42" t="s">
         <v>193</v>
@@ -2884,23 +2856,23 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.pathways</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.clinical_link_outs</v>
       </c>
       <c r="B43" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D43" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E43" t="s">
         <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="J43" t="s">
         <v>193</v>
@@ -2914,23 +2886,23 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" ref="A44" si="3">CONCATENATE(D44,".",F44)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.go_terms</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.sequence_link_outs</v>
       </c>
       <c r="B44" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D44" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E44" t="s">
         <v>85</v>
       </c>
       <c r="F44" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="J44" t="s">
         <v>193</v>
@@ -2944,30 +2916,27 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_within_lineage_comparisons</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>439</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.pathways</v>
+      </c>
+      <c r="B45" t="s">
+        <v>172</v>
       </c>
       <c r="C45" t="s">
-        <v>443</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E45" t="s">
         <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="J45" t="s">
         <v>193</v>
       </c>
-      <c r="K45">
-        <v>2</v>
-      </c>
       <c r="M45" t="s">
         <v>64</v>
       </c>
@@ -2977,30 +2946,27 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" ref="A46" si="4">CONCATENATE(D46,".",F46)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_across_lineage_comparisons</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>439</v>
+        <f t="shared" ref="A46" si="5">CONCATENATE(D46,".",F46)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.go_terms</v>
+      </c>
+      <c r="B46" t="s">
+        <v>172</v>
       </c>
       <c r="C46" t="s">
-        <v>443</v>
+        <v>173</v>
       </c>
       <c r="D46" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E46" t="s">
         <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="J46" t="s">
         <v>193</v>
       </c>
-      <c r="K46">
-        <v>3</v>
-      </c>
       <c r="M46" t="s">
         <v>64</v>
       </c>
@@ -3010,59 +2976,62 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_profiles</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_within_lineage_comparisons</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="C47" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D47" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E47" t="s">
         <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="J47" t="s">
         <v>193</v>
       </c>
       <c r="K47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M47" t="s">
         <v>64</v>
       </c>
+      <c r="N47" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" ref="A48:A53" si="5">CONCATENATE(D48,".",F48)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_lineage_comparisons</v>
+        <f t="shared" ref="A48" si="6">CONCATENATE(D48,".",F48)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_across_lineage_comparisons</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="C48" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="D48" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E48" t="s">
         <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>448</v>
+        <v>416</v>
       </c>
       <c r="J48" t="s">
         <v>193</v>
       </c>
       <c r="K48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M48" t="s">
         <v>64</v>
@@ -3073,86 +3042,86 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" ref="A49" si="6">CONCATENATE(D49,".",F49)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_treatment_comparisons</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_profiles</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="C49" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="D49" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E49" t="s">
         <v>85</v>
       </c>
       <c r="F49" t="s">
-        <v>449</v>
+        <v>417</v>
       </c>
       <c r="J49" t="s">
         <v>193</v>
       </c>
       <c r="K49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M49" t="s">
         <v>64</v>
       </c>
-      <c r="N49" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" si="5"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_profiles</v>
+        <f t="shared" ref="A50:A55" si="7">CONCATENATE(D50,".",F50)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_lineage_comparisons</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="C50" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="D50" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E50" t="s">
         <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="J50" t="s">
         <v>193</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M50" t="s">
         <v>64</v>
       </c>
+      <c r="N50" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f t="shared" si="5"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_genotype_comparisons</v>
+        <f t="shared" ref="A51" si="8">CONCATENATE(D51,".",F51)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_treatment_comparisons</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="C51" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="D51" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E51" t="s">
         <v>85</v>
       </c>
       <c r="F51" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="J51" t="s">
         <v>193</v>
@@ -3169,75 +3138,138 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>CONCATENATE(D52,".",F52)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_treatment_comparisons</v>
+        <f t="shared" si="7"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_profiles</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="C52" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="D52" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E52" t="s">
         <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>451</v>
+        <v>418</v>
       </c>
       <c r="J52" t="s">
         <v>193</v>
       </c>
       <c r="K52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M52" t="s">
         <v>64</v>
       </c>
-      <c r="N52" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" si="5"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_profiles</v>
+        <f t="shared" si="7"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_genotype_comparisons</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="C53" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="D53" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="E53" t="s">
         <v>85</v>
       </c>
       <c r="F53" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
       <c r="J53" t="s">
         <v>193</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M53" t="s">
         <v>64</v>
       </c>
+      <c r="N53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f>CONCATENATE(D54,".",F54)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_treatment_comparisons</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C54" t="s">
+        <v>437</v>
+      </c>
+      <c r="D54" t="s">
+        <v>420</v>
+      </c>
+      <c r="E54" t="s">
+        <v>85</v>
+      </c>
+      <c r="F54" t="s">
+        <v>441</v>
+      </c>
+      <c r="J54" t="s">
+        <v>193</v>
+      </c>
+      <c r="K54">
+        <v>2</v>
+      </c>
+      <c r="M54" t="s">
+        <v>64</v>
+      </c>
+      <c r="N54" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f t="shared" si="7"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_profiles</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C55" t="s">
+        <v>437</v>
+      </c>
+      <c r="D55" t="s">
+        <v>420</v>
+      </c>
+      <c r="E55" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" t="s">
+        <v>419</v>
+      </c>
+      <c r="J55" t="s">
+        <v>193</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="M55" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f t="shared" ref="A59:A60" si="7">CONCATENATE(D59,".",F59)</f>
+        <f t="shared" ref="A59:A60" si="9">CONCATENATE(D59,".",F59)</f>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.source_id</v>
       </c>
       <c r="B59" t="s">
@@ -3247,7 +3279,7 @@
         <v>156</v>
       </c>
       <c r="D59" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E59" t="s">
         <v>62</v>
@@ -3258,7 +3290,7 @@
       <c r="J59" t="s">
         <v>193</v>
       </c>
-      <c r="L59" t="s">
+      <c r="M59" t="s">
         <v>197</v>
       </c>
       <c r="N59" t="s">
@@ -3267,7 +3299,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.organism</v>
       </c>
       <c r="B60" t="s">
@@ -3277,7 +3309,7 @@
         <v>156</v>
       </c>
       <c r="D60" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E60" t="s">
         <v>62</v>
@@ -3313,7 +3345,7 @@
         <v>156</v>
       </c>
       <c r="D61" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E61" t="s">
         <v>62</v>
@@ -3339,7 +3371,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f t="shared" ref="A62" si="8">CONCATENATE(D62,".",F62)</f>
+        <f t="shared" ref="A62" si="10">CONCATENATE(D62,".",F62)</f>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.product</v>
       </c>
       <c r="B62" t="s">
@@ -3349,7 +3381,7 @@
         <v>156</v>
       </c>
       <c r="D62" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E62" t="s">
         <v>62</v>
@@ -3385,7 +3417,7 @@
         <v>156</v>
       </c>
       <c r="D63" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E63" t="s">
         <v>62</v>
@@ -3411,7 +3443,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f t="shared" ref="A64" si="9">CONCATENATE(D64,".",F64)</f>
+        <f t="shared" ref="A64" si="11">CONCATENATE(D64,".",F64)</f>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_type</v>
       </c>
       <c r="B64" t="s">
@@ -3421,7 +3453,7 @@
         <v>156</v>
       </c>
       <c r="D64" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E64" t="s">
         <v>62</v>
@@ -3457,7 +3489,7 @@
         <v>156</v>
       </c>
       <c r="D65" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E65" t="s">
         <v>62</v>
@@ -3480,7 +3512,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f t="shared" ref="A66:A67" si="10">CONCATENATE(D66,".",F66)</f>
+        <f t="shared" ref="A66:A67" si="12">CONCATENATE(D66,".",F66)</f>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_source_id</v>
       </c>
       <c r="B66" t="s">
@@ -3490,13 +3522,13 @@
         <v>156</v>
       </c>
       <c r="D66" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E66" t="s">
         <v>62</v>
       </c>
       <c r="F66" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="J66" t="s">
         <v>193</v>
@@ -3510,7 +3542,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_symbol</v>
       </c>
       <c r="B67" t="s">
@@ -3520,13 +3552,13 @@
         <v>156</v>
       </c>
       <c r="D67" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E67" t="s">
         <v>62</v>
       </c>
       <c r="F67" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="J67" t="s">
         <v>193</v>
@@ -3550,13 +3582,13 @@
         <v>162</v>
       </c>
       <c r="D68" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E68" t="s">
         <v>62</v>
       </c>
       <c r="F68" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="J68" t="s">
         <v>193</v>
@@ -3586,13 +3618,13 @@
         <v>162</v>
       </c>
       <c r="D69" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E69" t="s">
         <v>62</v>
       </c>
       <c r="F69" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="J69" t="s">
         <v>193</v>
@@ -3622,7 +3654,7 @@
         <v>162</v>
       </c>
       <c r="D70" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E70" t="s">
         <v>62</v>
@@ -3645,7 +3677,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f t="shared" ref="A71:A81" si="11">CONCATENATE(D71,".",F71)</f>
+        <f t="shared" ref="A71:A81" si="13">CONCATENATE(D71,".",F71)</f>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.strand</v>
       </c>
       <c r="B71" t="s">
@@ -3655,13 +3687,13 @@
         <v>162</v>
       </c>
       <c r="D71" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E71" t="s">
         <v>62</v>
       </c>
       <c r="F71" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="J71" t="s">
         <v>193</v>
@@ -3678,7 +3710,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.start_min</v>
       </c>
       <c r="B72" t="s">
@@ -3688,7 +3720,7 @@
         <v>175</v>
       </c>
       <c r="D72" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E72" t="s">
         <v>62</v>
@@ -3711,7 +3743,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.end_max</v>
       </c>
       <c r="B73" t="s">
@@ -3721,7 +3753,7 @@
         <v>175</v>
       </c>
       <c r="D73" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E73" t="s">
         <v>62</v>
@@ -3744,7 +3776,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_link_outs</v>
       </c>
       <c r="B74" t="s">
@@ -3754,13 +3786,13 @@
         <v>159</v>
       </c>
       <c r="D74" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E74" t="s">
         <v>85</v>
       </c>
       <c r="F74" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="J74" t="s">
         <v>193</v>
@@ -3774,7 +3806,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.protein_link_outs</v>
       </c>
       <c r="B75" t="s">
@@ -3784,13 +3816,13 @@
         <v>159</v>
       </c>
       <c r="D75" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E75" t="s">
         <v>85</v>
       </c>
       <c r="F75" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="J75" t="s">
         <v>193</v>
@@ -3804,7 +3836,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.clinical_link_outs</v>
       </c>
       <c r="B76" t="s">
@@ -3814,13 +3846,13 @@
         <v>159</v>
       </c>
       <c r="D76" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E76" t="s">
         <v>85</v>
       </c>
       <c r="F76" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="J76" t="s">
         <v>193</v>
@@ -3834,7 +3866,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.sequence_link_outs</v>
       </c>
       <c r="B77" t="s">
@@ -3844,13 +3876,13 @@
         <v>159</v>
       </c>
       <c r="D77" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E77" t="s">
         <v>85</v>
       </c>
       <c r="F77" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="J77" t="s">
         <v>193</v>
@@ -3864,7 +3896,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.pathways</v>
       </c>
       <c r="B78" t="s">
@@ -3874,13 +3906,13 @@
         <v>173</v>
       </c>
       <c r="D78" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E78" t="s">
         <v>85</v>
       </c>
       <c r="F78" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="J78" t="s">
         <v>193</v>
@@ -3894,7 +3926,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.go_terms</v>
       </c>
       <c r="B79" t="s">
@@ -3904,13 +3936,13 @@
         <v>173</v>
       </c>
       <c r="D79" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E79" t="s">
         <v>85</v>
       </c>
       <c r="F79" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="J79" t="s">
         <v>193</v>
@@ -3924,23 +3956,23 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_ptm</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C80" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="D80" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E80" t="s">
         <v>85</v>
       </c>
       <c r="F80" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="J80" t="s">
         <v>193</v>
@@ -3957,23 +3989,23 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_comparisons</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C81" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="D81" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="E81" t="s">
         <v>85</v>
       </c>
       <c r="F81" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="J81" t="s">
         <v>193</v>
@@ -3988,267 +4020,261 @@
         <v>65</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A157" cm="1">
-        <f t="array" aca="1" ref="A157" ca="1">157:184</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>398</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B85" t="s">
         <v>217</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C85" t="s">
         <v>397</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D85" t="s">
         <v>249</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E85" t="s">
         <v>85</v>
       </c>
-      <c r="F160" t="s">
+      <c r="F85" t="s">
         <v>397</v>
       </c>
-      <c r="G160" t="s">
+      <c r="G85" t="s">
         <v>248</v>
       </c>
-      <c r="H160" t="s">
+      <c r="H85" t="s">
         <v>248</v>
       </c>
-      <c r="I160" t="s">
+      <c r="I85" t="s">
         <v>248</v>
       </c>
-      <c r="J160" t="s">
+      <c r="J85" t="s">
         <v>248</v>
       </c>
-      <c r="K160" t="s">
+      <c r="K85" t="s">
         <v>248</v>
       </c>
-      <c r="L160" t="s">
+      <c r="L85" t="s">
         <v>66</v>
       </c>
-      <c r="M160" t="s">
+      <c r="M85" t="s">
         <v>64</v>
       </c>
-      <c r="N160" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="N85" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>405</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B86" t="s">
         <v>217</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C86" t="s">
         <v>404</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D86" t="s">
         <v>249</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E86" t="s">
         <v>85</v>
       </c>
-      <c r="F161" t="s">
+      <c r="F86" t="s">
         <v>404</v>
       </c>
-      <c r="G161" t="s">
+      <c r="G86" t="s">
         <v>248</v>
       </c>
-      <c r="H161" t="s">
+      <c r="H86" t="s">
         <v>248</v>
       </c>
-      <c r="I161" t="s">
+      <c r="I86" t="s">
         <v>248</v>
       </c>
-      <c r="J161" t="s">
+      <c r="J86" t="s">
         <v>248</v>
       </c>
-      <c r="K161" t="s">
+      <c r="K86" t="s">
         <v>248</v>
       </c>
-      <c r="M161" t="s">
+      <c r="M86" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>389</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B87" t="s">
         <v>204</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C87" t="s">
         <v>399</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D87" t="s">
         <v>249</v>
       </c>
-      <c r="E162" t="s">
-        <v>62</v>
-      </c>
-      <c r="F162" t="s">
+      <c r="E87" t="s">
+        <v>62</v>
+      </c>
+      <c r="F87" t="s">
         <v>390</v>
       </c>
-      <c r="L162" t="s">
+      <c r="L87" t="s">
         <v>66</v>
       </c>
-      <c r="M162" t="s">
+      <c r="M87" t="s">
         <v>64</v>
       </c>
-      <c r="N162" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="N87" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>391</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B88" t="s">
         <v>204</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C88" t="s">
         <v>399</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D88" t="s">
         <v>249</v>
       </c>
-      <c r="E163" t="s">
-        <v>62</v>
-      </c>
-      <c r="F163" t="s">
+      <c r="E88" t="s">
+        <v>62</v>
+      </c>
+      <c r="F88" t="s">
         <v>392</v>
       </c>
-      <c r="L163" t="s">
+      <c r="L88" t="s">
         <v>66</v>
       </c>
-      <c r="M163" t="s">
+      <c r="M88" t="s">
         <v>64</v>
       </c>
-      <c r="N163" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="N88" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>393</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B89" t="s">
         <v>204</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C89" t="s">
         <v>399</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D89" t="s">
         <v>249</v>
       </c>
-      <c r="E164" t="s">
-        <v>62</v>
-      </c>
-      <c r="F164" t="s">
+      <c r="E89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F89" t="s">
         <v>395</v>
       </c>
-      <c r="L164" t="s">
+      <c r="L89" t="s">
         <v>66</v>
       </c>
-      <c r="M164" t="s">
+      <c r="M89" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>394</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B90" t="s">
         <v>204</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C90" t="s">
         <v>399</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D90" t="s">
         <v>249</v>
       </c>
-      <c r="E165" t="s">
-        <v>62</v>
-      </c>
-      <c r="F165" t="s">
+      <c r="E90" t="s">
+        <v>62</v>
+      </c>
+      <c r="F90" t="s">
         <v>396</v>
       </c>
-      <c r="L165" t="s">
+      <c r="L90" t="s">
         <v>66</v>
       </c>
-      <c r="M165" t="s">
+      <c r="M90" t="s">
         <v>64</v>
       </c>
-      <c r="N165" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="N90" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>400</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B91" t="s">
         <v>204</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C91" t="s">
         <v>399</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D91" t="s">
         <v>249</v>
       </c>
-      <c r="E166" t="s">
-        <v>62</v>
-      </c>
-      <c r="F166" t="s">
+      <c r="E91" t="s">
+        <v>62</v>
+      </c>
+      <c r="F91" t="s">
         <v>401</v>
       </c>
-      <c r="L166" t="s">
+      <c r="L91" t="s">
         <v>66</v>
       </c>
-      <c r="M166" t="s">
+      <c r="M91" t="s">
         <v>64</v>
       </c>
-      <c r="N166" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="N91" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>402</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B92" t="s">
         <v>204</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C92" t="s">
         <v>399</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D92" t="s">
         <v>249</v>
       </c>
-      <c r="E167" t="s">
-        <v>62</v>
-      </c>
-      <c r="F167" t="s">
+      <c r="E92" t="s">
+        <v>62</v>
+      </c>
+      <c r="F92" t="s">
         <v>403</v>
       </c>
-      <c r="L167" t="s">
+      <c r="L92" t="s">
         <v>66</v>
       </c>
-      <c r="M167" t="s">
+      <c r="M92" t="s">
         <v>64</v>
       </c>
-      <c r="N167" t="s">
+      <c r="N92" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5771,8 +5797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0452A-4FB9-4500-9B58-DC3A1BF00BD2}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6048,7 +6074,7 @@
         <v>184</v>
       </c>
       <c r="D20">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -6669,13 +6695,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="C65" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D65">
         <v>900</v>
@@ -6683,13 +6709,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="C66" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="D66">
         <v>901</v>
@@ -6697,13 +6723,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="C67" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="D67">
         <v>902</v>
@@ -6711,13 +6737,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="C68" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="D68">
         <v>950</v>

</xml_diff>

<commit_message>
genome browser track mods, feature lookup service, prod-like expression profiles
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\ErythronDBWebsite\Model\lib\wdk\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A334B3-22EF-49E5-96B6-179EB96F4AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCC5EFB-BF6F-488F-8236-F47DDDD28C2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="commonIndividuals" localSheetId="3">common!$A$1:$N$36</definedName>
-    <definedName name="individuals" localSheetId="0">individuals!$A$1:$N$59</definedName>
+    <definedName name="individuals" localSheetId="0">individuals!$A$1:$N$62</definedName>
     <definedName name="individuals" localSheetId="1">orthomcl!$A$1:$N$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="461">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1329,9 +1329,6 @@
     <t>DatasetRecordClasses.DatasetRecordClass.Searches</t>
   </si>
   <si>
-    <t>Study005.study005_expression</t>
-  </si>
-  <si>
     <t>## Mouse Gene Attributes ##</t>
   </si>
   <si>
@@ -1362,15 +1359,6 @@
     <t>study001_across_lineage_comparisons</t>
   </si>
   <si>
-    <t>study001_profiles</t>
-  </si>
-  <si>
-    <t>study002_profiles</t>
-  </si>
-  <si>
-    <t>study005_profiles</t>
-  </si>
-  <si>
     <t>MouseGeneRecordClasses.MouseGeneRecordClass</t>
   </si>
   <si>
@@ -1467,9 +1455,6 @@
     <t>study003_questions.study003_comparison</t>
   </si>
   <si>
-    <t>Attributes ##</t>
-  </si>
-  <si>
     <t>study001_questions.study001_comparison</t>
   </si>
   <si>
@@ -1486,6 +1471,27 @@
   </si>
   <si>
     <t>study005_questions.study005_expression</t>
+  </si>
+  <si>
+    <t>DatasetRecordClasses.DatasetRecordClass.primary_publication_pubmed_url</t>
+  </si>
+  <si>
+    <t>study001_gene_profiles</t>
+  </si>
+  <si>
+    <t>study001_reporter_profiles</t>
+  </si>
+  <si>
+    <t>study005_reporter_profiles</t>
+  </si>
+  <si>
+    <t>study005_gene_profiles</t>
+  </si>
+  <si>
+    <t>study002_reporter_profiles</t>
+  </si>
+  <si>
+    <t>study002_gene_profiles</t>
   </si>
 </sst>
 </file>
@@ -1816,13 +1822,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N92"/>
+  <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1964,13 +1970,13 @@
         <v>156</v>
       </c>
       <c r="D10" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
@@ -1978,7 +1984,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" ref="A11:A22" si="0">CONCATENATE(D11,".",F11)</f>
+        <f t="shared" ref="A11:A21" si="0">CONCATENATE(D11,".",F11)</f>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.MouseGeneQuestions.upload</v>
       </c>
       <c r="B11" t="s">
@@ -1988,13 +1994,13 @@
         <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="L11" t="s">
         <v>27</v>
@@ -2012,13 +2018,13 @@
         <v>156</v>
       </c>
       <c r="D12" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="L12" t="s">
         <v>27</v>
@@ -2036,13 +2042,13 @@
         <v>156</v>
       </c>
       <c r="D13" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="L13" t="s">
         <v>27</v>
@@ -2060,13 +2066,13 @@
         <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="L14" t="s">
         <v>27</v>
@@ -2084,13 +2090,13 @@
         <v>156</v>
       </c>
       <c r="D15" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="L15" t="s">
         <v>27</v>
@@ -2102,19 +2108,19 @@
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_questions.study003_comparison</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C16" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D16" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="L16" t="s">
         <v>27</v>
@@ -2126,19 +2132,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_comparison</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C17" t="s">
         <v>429</v>
       </c>
-      <c r="C17" t="s">
-        <v>433</v>
-      </c>
       <c r="D17" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2153,19 +2159,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_expression</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C18" t="s">
         <v>429</v>
       </c>
-      <c r="C18" t="s">
-        <v>433</v>
-      </c>
       <c r="D18" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="K18">
         <v>2</v>
@@ -2180,19 +2186,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_comparison</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C19" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D19" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="K19">
         <v>3</v>
@@ -2207,19 +2213,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_expression</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C20" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D20" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="K20">
         <v>4</v>
@@ -2234,19 +2240,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_comparison</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C21" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D21" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="K21">
         <v>5</v>
@@ -2261,19 +2267,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_expression</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C22" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D22" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="K22">
         <v>6</v>
@@ -2284,7 +2290,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2299,7 +2305,7 @@
         <v>156</v>
       </c>
       <c r="D26" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E26" t="s">
         <v>62</v>
@@ -2319,7 +2325,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" ref="A27:A49" si="3">CONCATENATE(D27,".",F27)</f>
+        <f t="shared" ref="A27:A47" si="3">CONCATENATE(D27,".",F27)</f>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.organism</v>
       </c>
       <c r="B27" t="s">
@@ -2329,7 +2335,7 @@
         <v>156</v>
       </c>
       <c r="D27" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E27" t="s">
         <v>62</v>
@@ -2365,7 +2371,7 @@
         <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E28" t="s">
         <v>62</v>
@@ -2401,7 +2407,7 @@
         <v>156</v>
       </c>
       <c r="D29" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E29" t="s">
         <v>62</v>
@@ -2437,7 +2443,7 @@
         <v>156</v>
       </c>
       <c r="D30" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E30" t="s">
         <v>62</v>
@@ -2473,7 +2479,7 @@
         <v>156</v>
       </c>
       <c r="D31" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E31" t="s">
         <v>62</v>
@@ -2509,7 +2515,7 @@
         <v>156</v>
       </c>
       <c r="D32" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E32" t="s">
         <v>62</v>
@@ -2542,13 +2548,13 @@
         <v>156</v>
       </c>
       <c r="D33" t="s">
+        <v>416</v>
+      </c>
+      <c r="E33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" t="s">
         <v>420</v>
-      </c>
-      <c r="E33" t="s">
-        <v>62</v>
-      </c>
-      <c r="F33" t="s">
-        <v>424</v>
       </c>
       <c r="J33" t="s">
         <v>193</v>
@@ -2572,13 +2578,13 @@
         <v>156</v>
       </c>
       <c r="D34" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E34" t="s">
         <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="J34" t="s">
         <v>193</v>
@@ -2602,13 +2608,13 @@
         <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E35" t="s">
         <v>62</v>
       </c>
       <c r="F35" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="J35" t="s">
         <v>193</v>
@@ -2638,13 +2644,13 @@
         <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E36" t="s">
         <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="J36" t="s">
         <v>193</v>
@@ -2674,7 +2680,7 @@
         <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E37" t="s">
         <v>62</v>
@@ -2707,13 +2713,13 @@
         <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E38" t="s">
         <v>62</v>
       </c>
       <c r="F38" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="J38" t="s">
         <v>193</v>
@@ -2740,7 +2746,7 @@
         <v>175</v>
       </c>
       <c r="D39" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E39" t="s">
         <v>62</v>
@@ -2773,7 +2779,7 @@
         <v>175</v>
       </c>
       <c r="D40" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E40" t="s">
         <v>62</v>
@@ -2806,13 +2812,13 @@
         <v>159</v>
       </c>
       <c r="D41" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E41" t="s">
         <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J41" t="s">
         <v>193</v>
@@ -2836,13 +2842,13 @@
         <v>159</v>
       </c>
       <c r="D42" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E42" t="s">
         <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J42" t="s">
         <v>193</v>
@@ -2866,13 +2872,13 @@
         <v>159</v>
       </c>
       <c r="D43" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E43" t="s">
         <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J43" t="s">
         <v>193</v>
@@ -2896,13 +2902,13 @@
         <v>159</v>
       </c>
       <c r="D44" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E44" t="s">
         <v>85</v>
       </c>
       <c r="F44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J44" t="s">
         <v>193</v>
@@ -2926,13 +2932,13 @@
         <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E45" t="s">
         <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J45" t="s">
         <v>193</v>
@@ -2956,13 +2962,13 @@
         <v>173</v>
       </c>
       <c r="D46" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E46" t="s">
         <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J46" t="s">
         <v>193</v>
@@ -2980,25 +2986,25 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_within_lineage_comparisons</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C47" t="s">
         <v>429</v>
       </c>
-      <c r="C47" t="s">
-        <v>433</v>
-      </c>
       <c r="D47" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E47" t="s">
         <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J47" t="s">
         <v>193</v>
       </c>
       <c r="K47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M47" t="s">
         <v>64</v>
@@ -3009,29 +3015,29 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" ref="A48" si="6">CONCATENATE(D48,".",F48)</f>
+        <f t="shared" ref="A48:A51" si="6">CONCATENATE(D48,".",F48)</f>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_across_lineage_comparisons</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C48" t="s">
         <v>429</v>
       </c>
-      <c r="C48" t="s">
-        <v>433</v>
-      </c>
       <c r="D48" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E48" t="s">
         <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J48" t="s">
         <v>193</v>
       </c>
       <c r="K48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M48" t="s">
         <v>64</v>
@@ -3042,29 +3048,29 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_profiles</v>
+        <f>CONCATENATE(D49,".",F49)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_reporter_profiles</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C49" t="s">
         <v>429</v>
       </c>
-      <c r="C49" t="s">
-        <v>433</v>
-      </c>
       <c r="D49" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E49" t="s">
         <v>85</v>
       </c>
       <c r="F49" t="s">
-        <v>417</v>
+        <v>456</v>
       </c>
       <c r="J49" t="s">
         <v>193</v>
       </c>
       <c r="K49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M49" t="s">
         <v>64</v>
@@ -3072,62 +3078,59 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" ref="A50:A55" si="7">CONCATENATE(D50,".",F50)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_lineage_comparisons</v>
+        <f t="shared" si="6"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_gene_profiles</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C50" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D50" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E50" t="s">
         <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
       <c r="J50" t="s">
         <v>193</v>
       </c>
       <c r="K50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M50" t="s">
         <v>64</v>
       </c>
-      <c r="N50" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f t="shared" ref="A51" si="8">CONCATENATE(D51,".",F51)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_treatment_comparisons</v>
+        <f t="shared" si="6"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_lineage_comparisons</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C51" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D51" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E51" t="s">
         <v>85</v>
       </c>
       <c r="F51" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="J51" t="s">
         <v>193</v>
       </c>
       <c r="K51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M51" t="s">
         <v>64</v>
@@ -3138,53 +3141,56 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f t="shared" si="7"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_profiles</v>
+        <f t="shared" ref="A52" si="7">CONCATENATE(D52,".",F52)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_treatment_comparisons</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C52" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D52" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E52" t="s">
         <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>418</v>
+        <v>435</v>
       </c>
       <c r="J52" t="s">
         <v>193</v>
       </c>
       <c r="K52">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M52" t="s">
         <v>64</v>
       </c>
+      <c r="N52" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" si="7"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_genotype_comparisons</v>
+        <f t="shared" ref="A53:A57" si="8">CONCATENATE(D53,".",F53)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_reporter_profiles</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="C53" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="D53" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E53" t="s">
         <v>85</v>
       </c>
       <c r="F53" t="s">
-        <v>440</v>
+        <v>459</v>
       </c>
       <c r="J53" t="s">
         <v>193</v>
@@ -3195,184 +3201,172 @@
       <c r="M53" t="s">
         <v>64</v>
       </c>
-      <c r="N53" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f>CONCATENATE(D54,".",F54)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_treatment_comparisons</v>
+        <f t="shared" ref="A54" si="9">CONCATENATE(D54,".",F54)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_gene_profiles</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="C54" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="D54" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E54" t="s">
         <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>441</v>
+        <v>460</v>
       </c>
       <c r="J54" t="s">
         <v>193</v>
       </c>
       <c r="K54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M54" t="s">
         <v>64</v>
       </c>
-      <c r="N54" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f t="shared" si="7"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_profiles</v>
+        <f t="shared" si="8"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_genotype_comparisons</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C55" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D55" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E55" t="s">
         <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>419</v>
+        <v>436</v>
       </c>
       <c r="J55" t="s">
         <v>193</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M55" t="s">
         <v>64</v>
       </c>
+      <c r="N55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f>CONCATENATE(D56,".",F56)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_treatment_comparisons</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C56" t="s">
+        <v>433</v>
+      </c>
+      <c r="D56" t="s">
+        <v>416</v>
+      </c>
+      <c r="E56" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" t="s">
+        <v>437</v>
+      </c>
+      <c r="J56" t="s">
+        <v>193</v>
+      </c>
+      <c r="K56">
+        <v>3</v>
+      </c>
+      <c r="M56" t="s">
+        <v>64</v>
+      </c>
+      <c r="N56" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
-        <f t="shared" ref="A59:A60" si="9">CONCATENATE(D59,".",F59)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.source_id</v>
-      </c>
-      <c r="B59" t="s">
-        <v>155</v>
-      </c>
-      <c r="C59" t="s">
-        <v>156</v>
-      </c>
-      <c r="D59" t="s">
-        <v>442</v>
-      </c>
-      <c r="E59" t="s">
-        <v>62</v>
-      </c>
-      <c r="F59" t="s">
-        <v>127</v>
-      </c>
-      <c r="J59" t="s">
+      <c r="A57" t="str">
+        <f t="shared" si="8"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_reporter_profiles</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C57" t="s">
+        <v>433</v>
+      </c>
+      <c r="D57" t="s">
+        <v>416</v>
+      </c>
+      <c r="E57" t="s">
+        <v>85</v>
+      </c>
+      <c r="F57" t="s">
+        <v>457</v>
+      </c>
+      <c r="J57" t="s">
         <v>193</v>
       </c>
-      <c r="M59" t="s">
-        <v>197</v>
-      </c>
-      <c r="N59" t="s">
-        <v>65</v>
+      <c r="K57">
+        <v>2</v>
+      </c>
+      <c r="M57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f t="shared" ref="A58" si="10">CONCATENATE(D58,".",F58)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_gene_profiles</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C58" t="s">
+        <v>433</v>
+      </c>
+      <c r="D58" t="s">
+        <v>416</v>
+      </c>
+      <c r="E58" t="s">
+        <v>85</v>
+      </c>
+      <c r="F58" t="s">
+        <v>458</v>
+      </c>
+      <c r="J58" t="s">
+        <v>193</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="M58" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="str">
-        <f t="shared" si="9"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.organism</v>
-      </c>
-      <c r="B60" t="s">
-        <v>155</v>
-      </c>
-      <c r="C60" t="s">
-        <v>156</v>
-      </c>
-      <c r="D60" t="s">
-        <v>442</v>
-      </c>
-      <c r="E60" t="s">
-        <v>62</v>
-      </c>
-      <c r="F60" t="s">
-        <v>396</v>
-      </c>
-      <c r="J60" t="s">
-        <v>193</v>
-      </c>
-      <c r="K60">
-        <v>1</v>
-      </c>
-      <c r="L60" t="s">
-        <v>66</v>
-      </c>
-      <c r="M60" t="s">
-        <v>197</v>
-      </c>
-      <c r="N60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="str">
-        <f>CONCATENATE(D61,".",F61)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.symbol</v>
-      </c>
-      <c r="B61" t="s">
-        <v>155</v>
-      </c>
-      <c r="C61" t="s">
-        <v>156</v>
-      </c>
-      <c r="D61" t="s">
-        <v>442</v>
-      </c>
-      <c r="E61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F61" t="s">
-        <v>243</v>
-      </c>
-      <c r="J61" t="s">
-        <v>193</v>
-      </c>
-      <c r="K61">
-        <v>2</v>
-      </c>
-      <c r="L61" t="s">
-        <v>66</v>
-      </c>
-      <c r="M61" t="s">
-        <v>197</v>
-      </c>
-      <c r="N61" t="s">
-        <v>65</v>
+      <c r="A60" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f t="shared" ref="A62" si="10">CONCATENATE(D62,".",F62)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.product</v>
+        <f t="shared" ref="A62:A63" si="11">CONCATENATE(D62,".",F62)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.source_id</v>
       </c>
       <c r="B62" t="s">
         <v>155</v>
@@ -3381,23 +3375,17 @@
         <v>156</v>
       </c>
       <c r="D62" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E62" t="s">
         <v>62</v>
       </c>
       <c r="F62" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J62" t="s">
         <v>193</v>
       </c>
-      <c r="K62">
-        <v>3</v>
-      </c>
-      <c r="L62" t="s">
-        <v>66</v>
-      </c>
       <c r="M62" t="s">
         <v>197</v>
       </c>
@@ -3407,8 +3395,8 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f>CONCATENATE(D63,".",F63)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.synonym</v>
+        <f t="shared" si="11"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.organism</v>
       </c>
       <c r="B63" t="s">
         <v>155</v>
@@ -3417,19 +3405,19 @@
         <v>156</v>
       </c>
       <c r="D63" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E63" t="s">
         <v>62</v>
       </c>
       <c r="F63" t="s">
-        <v>244</v>
+        <v>396</v>
       </c>
       <c r="J63" t="s">
         <v>193</v>
       </c>
       <c r="K63">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L63" t="s">
         <v>66</v>
@@ -3443,8 +3431,8 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f t="shared" ref="A64" si="11">CONCATENATE(D64,".",F64)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_type</v>
+        <f>CONCATENATE(D64,".",F64)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.symbol</v>
       </c>
       <c r="B64" t="s">
         <v>155</v>
@@ -3453,19 +3441,19 @@
         <v>156</v>
       </c>
       <c r="D64" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E64" t="s">
         <v>62</v>
       </c>
       <c r="F64" t="s">
-        <v>209</v>
+        <v>243</v>
       </c>
       <c r="J64" t="s">
         <v>193</v>
       </c>
       <c r="K64">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L64" t="s">
         <v>66</v>
@@ -3479,8 +3467,8 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f>CONCATENATE(D65,".",F65)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_record_link</v>
+        <f t="shared" ref="A65" si="12">CONCATENATE(D65,".",F65)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.product</v>
       </c>
       <c r="B65" t="s">
         <v>155</v>
@@ -3489,19 +3477,19 @@
         <v>156</v>
       </c>
       <c r="D65" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E65" t="s">
         <v>62</v>
       </c>
       <c r="F65" t="s">
-        <v>242</v>
+        <v>131</v>
       </c>
       <c r="J65" t="s">
         <v>193</v>
       </c>
       <c r="K65">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L65" t="s">
         <v>66</v>
@@ -3509,11 +3497,14 @@
       <c r="M65" t="s">
         <v>197</v>
       </c>
+      <c r="N65" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f t="shared" ref="A66:A67" si="12">CONCATENATE(D66,".",F66)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_source_id</v>
+        <f>CONCATENATE(D66,".",F66)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.synonym</v>
       </c>
       <c r="B66" t="s">
         <v>155</v>
@@ -3522,19 +3513,25 @@
         <v>156</v>
       </c>
       <c r="D66" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E66" t="s">
         <v>62</v>
       </c>
       <c r="F66" t="s">
-        <v>424</v>
+        <v>244</v>
       </c>
       <c r="J66" t="s">
         <v>193</v>
       </c>
       <c r="K66">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="L66" t="s">
+        <v>66</v>
+      </c>
+      <c r="M66" t="s">
+        <v>197</v>
       </c>
       <c r="N66" t="s">
         <v>65</v>
@@ -3542,8 +3539,8 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f t="shared" si="12"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_symbol</v>
+        <f t="shared" ref="A67" si="13">CONCATENATE(D67,".",F67)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_type</v>
       </c>
       <c r="B67" t="s">
         <v>155</v>
@@ -3552,19 +3549,25 @@
         <v>156</v>
       </c>
       <c r="D67" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E67" t="s">
         <v>62</v>
       </c>
       <c r="F67" t="s">
-        <v>425</v>
+        <v>209</v>
       </c>
       <c r="J67" t="s">
         <v>193</v>
       </c>
       <c r="K67">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="L67" t="s">
+        <v>66</v>
+      </c>
+      <c r="M67" t="s">
+        <v>197</v>
       </c>
       <c r="N67" t="s">
         <v>65</v>
@@ -3573,28 +3576,28 @@
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>CONCATENATE(D68,".",F68)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.locus</v>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_record_link</v>
       </c>
       <c r="B68" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C68" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D68" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E68" t="s">
         <v>62</v>
       </c>
       <c r="F68" t="s">
-        <v>422</v>
+        <v>242</v>
       </c>
       <c r="J68" t="s">
         <v>193</v>
       </c>
       <c r="K68">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L68" t="s">
         <v>66</v>
@@ -3602,41 +3605,32 @@
       <c r="M68" t="s">
         <v>197</v>
       </c>
-      <c r="N68" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f>CONCATENATE(D69,".",F69)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.location</v>
+        <f t="shared" ref="A69:A70" si="14">CONCATENATE(D69,".",F69)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_source_id</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C69" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D69" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E69" t="s">
         <v>62</v>
       </c>
       <c r="F69" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="J69" t="s">
         <v>193</v>
       </c>
       <c r="K69">
-        <v>2</v>
-      </c>
-      <c r="L69" t="s">
-        <v>66</v>
-      </c>
-      <c r="M69" t="s">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="N69" t="s">
         <v>65</v>
@@ -3644,32 +3638,29 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f>CONCATENATE(D70,".",F70)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.chromosome</v>
+        <f t="shared" si="14"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_symbol</v>
       </c>
       <c r="B70" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C70" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D70" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E70" t="s">
         <v>62</v>
       </c>
       <c r="F70" t="s">
-        <v>208</v>
+        <v>421</v>
       </c>
       <c r="J70" t="s">
         <v>193</v>
       </c>
-      <c r="L70" t="s">
-        <v>66</v>
-      </c>
-      <c r="M70" t="s">
-        <v>197</v>
+      <c r="K70">
+        <v>6</v>
       </c>
       <c r="N70" t="s">
         <v>65</v>
@@ -3677,8 +3668,8 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f t="shared" ref="A71:A81" si="13">CONCATENATE(D71,".",F71)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.strand</v>
+        <f>CONCATENATE(D71,".",F71)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.locus</v>
       </c>
       <c r="B71" t="s">
         <v>162</v>
@@ -3687,17 +3678,20 @@
         <v>162</v>
       </c>
       <c r="D71" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E71" t="s">
         <v>62</v>
       </c>
       <c r="F71" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="J71" t="s">
         <v>193</v>
       </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
       <c r="L71" t="s">
         <v>66</v>
       </c>
@@ -3710,27 +3704,30 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.start_min</v>
+        <f>CONCATENATE(D72,".",F72)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.location</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C72" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="D72" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E72" t="s">
         <v>62</v>
       </c>
       <c r="F72" t="s">
-        <v>206</v>
+        <v>419</v>
       </c>
       <c r="J72" t="s">
         <v>193</v>
       </c>
+      <c r="K72">
+        <v>2</v>
+      </c>
       <c r="L72" t="s">
         <v>66</v>
       </c>
@@ -3743,23 +3740,23 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.end_max</v>
+        <f>CONCATENATE(D73,".",F73)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.chromosome</v>
       </c>
       <c r="B73" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C73" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="D73" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E73" t="s">
         <v>62</v>
       </c>
       <c r="F73" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J73" t="s">
         <v>193</v>
@@ -3776,29 +3773,32 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_link_outs</v>
+        <f t="shared" ref="A74:A84" si="15">CONCATENATE(D74,".",F74)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.strand</v>
       </c>
       <c r="B74" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C74" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D74" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E74" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="F74" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="J74" t="s">
         <v>193</v>
       </c>
+      <c r="L74" t="s">
+        <v>66</v>
+      </c>
       <c r="M74" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="N74" t="s">
         <v>65</v>
@@ -3806,29 +3806,32 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.protein_link_outs</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.start_min</v>
       </c>
       <c r="B75" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="C75" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E75" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="F75" t="s">
-        <v>410</v>
+        <v>206</v>
       </c>
       <c r="J75" t="s">
         <v>193</v>
       </c>
+      <c r="L75" t="s">
+        <v>66</v>
+      </c>
       <c r="M75" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="N75" t="s">
         <v>65</v>
@@ -3836,29 +3839,32 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.clinical_link_outs</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.end_max</v>
       </c>
       <c r="B76" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="C76" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="D76" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E76" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="F76" t="s">
-        <v>411</v>
+        <v>207</v>
       </c>
       <c r="J76" t="s">
         <v>193</v>
       </c>
+      <c r="L76" t="s">
+        <v>66</v>
+      </c>
       <c r="M76" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="N76" t="s">
         <v>65</v>
@@ -3866,8 +3872,8 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.sequence_link_outs</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_link_outs</v>
       </c>
       <c r="B77" t="s">
         <v>157</v>
@@ -3876,13 +3882,13 @@
         <v>159</v>
       </c>
       <c r="D77" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E77" t="s">
         <v>85</v>
       </c>
       <c r="F77" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="J77" t="s">
         <v>193</v>
@@ -3896,23 +3902,23 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.pathways</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.protein_link_outs</v>
       </c>
       <c r="B78" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C78" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D78" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E78" t="s">
         <v>85</v>
       </c>
       <c r="F78" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="J78" t="s">
         <v>193</v>
@@ -3926,23 +3932,23 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.go_terms</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.clinical_link_outs</v>
       </c>
       <c r="B79" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C79" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D79" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E79" t="s">
         <v>85</v>
       </c>
       <c r="F79" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="J79" t="s">
         <v>193</v>
@@ -3956,30 +3962,27 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_ptm</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>431</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.sequence_link_outs</v>
+      </c>
+      <c r="B80" t="s">
+        <v>157</v>
       </c>
       <c r="C80" t="s">
-        <v>436</v>
+        <v>159</v>
       </c>
       <c r="D80" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E80" t="s">
         <v>85</v>
       </c>
       <c r="F80" t="s">
-        <v>443</v>
+        <v>411</v>
       </c>
       <c r="J80" t="s">
         <v>193</v>
       </c>
-      <c r="K80">
-        <v>1</v>
-      </c>
       <c r="M80" t="s">
         <v>64</v>
       </c>
@@ -3989,30 +3992,27 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f t="shared" si="13"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_comparisons</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>431</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.pathways</v>
+      </c>
+      <c r="B81" t="s">
+        <v>172</v>
       </c>
       <c r="C81" t="s">
-        <v>436</v>
+        <v>173</v>
       </c>
       <c r="D81" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E81" t="s">
         <v>85</v>
       </c>
       <c r="F81" t="s">
-        <v>444</v>
+        <v>413</v>
       </c>
       <c r="J81" t="s">
         <v>193</v>
       </c>
-      <c r="K81">
-        <v>2</v>
-      </c>
       <c r="M81" t="s">
         <v>64</v>
       </c>
@@ -4020,140 +4020,140 @@
         <v>65</v>
       </c>
     </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" t="str">
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.go_terms</v>
+      </c>
+      <c r="B82" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" t="s">
+        <v>173</v>
+      </c>
+      <c r="D82" t="s">
+        <v>438</v>
+      </c>
+      <c r="E82" t="s">
+        <v>85</v>
+      </c>
+      <c r="F82" t="s">
+        <v>412</v>
+      </c>
+      <c r="J82" t="s">
+        <v>193</v>
+      </c>
+      <c r="M82" t="s">
+        <v>64</v>
+      </c>
+      <c r="N82" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>398</v>
-      </c>
-      <c r="B85" t="s">
-        <v>217</v>
-      </c>
-      <c r="C85" t="s">
-        <v>397</v>
-      </c>
-      <c r="D85" t="s">
-        <v>249</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="A83" t="str">
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_ptm</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C83" t="s">
+        <v>432</v>
+      </c>
+      <c r="D83" t="s">
+        <v>438</v>
+      </c>
+      <c r="E83" t="s">
         <v>85</v>
       </c>
-      <c r="F85" t="s">
-        <v>397</v>
-      </c>
-      <c r="G85" t="s">
-        <v>248</v>
-      </c>
-      <c r="H85" t="s">
-        <v>248</v>
-      </c>
-      <c r="I85" t="s">
-        <v>248</v>
-      </c>
-      <c r="J85" t="s">
-        <v>248</v>
-      </c>
-      <c r="K85" t="s">
-        <v>248</v>
-      </c>
-      <c r="L85" t="s">
-        <v>66</v>
-      </c>
-      <c r="M85" t="s">
+      <c r="F83" t="s">
+        <v>439</v>
+      </c>
+      <c r="J83" t="s">
+        <v>193</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="M83" t="s">
         <v>64</v>
       </c>
-      <c r="N85" t="s">
+      <c r="N83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_comparisons</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C84" t="s">
+        <v>432</v>
+      </c>
+      <c r="D84" t="s">
+        <v>438</v>
+      </c>
+      <c r="E84" t="s">
+        <v>85</v>
+      </c>
+      <c r="F84" t="s">
+        <v>440</v>
+      </c>
+      <c r="J84" t="s">
+        <v>193</v>
+      </c>
+      <c r="K84">
+        <v>2</v>
+      </c>
+      <c r="M84" t="s">
+        <v>64</v>
+      </c>
+      <c r="N84" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>405</v>
-      </c>
-      <c r="B86" t="s">
-        <v>217</v>
-      </c>
-      <c r="C86" t="s">
-        <v>404</v>
-      </c>
-      <c r="D86" t="s">
-        <v>249</v>
-      </c>
-      <c r="E86" t="s">
-        <v>85</v>
-      </c>
-      <c r="F86" t="s">
-        <v>404</v>
-      </c>
-      <c r="G86" t="s">
-        <v>248</v>
-      </c>
-      <c r="H86" t="s">
-        <v>248</v>
-      </c>
-      <c r="I86" t="s">
-        <v>248</v>
-      </c>
-      <c r="J86" t="s">
-        <v>248</v>
-      </c>
-      <c r="K86" t="s">
-        <v>248</v>
-      </c>
-      <c r="M86" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>389</v>
-      </c>
-      <c r="B87" t="s">
-        <v>204</v>
-      </c>
-      <c r="C87" t="s">
-        <v>399</v>
-      </c>
-      <c r="D87" t="s">
-        <v>249</v>
-      </c>
-      <c r="E87" t="s">
-        <v>62</v>
-      </c>
-      <c r="F87" t="s">
-        <v>390</v>
-      </c>
-      <c r="L87" t="s">
-        <v>66</v>
-      </c>
-      <c r="M87" t="s">
-        <v>64</v>
-      </c>
-      <c r="N87" t="s">
-        <v>65</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="B88" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="C88" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D88" t="s">
         <v>249</v>
       </c>
       <c r="E88" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F88" t="s">
-        <v>392</v>
+        <v>397</v>
+      </c>
+      <c r="G88" t="s">
+        <v>248</v>
+      </c>
+      <c r="H88" t="s">
+        <v>248</v>
+      </c>
+      <c r="I88" t="s">
+        <v>248</v>
+      </c>
+      <c r="J88" t="s">
+        <v>248</v>
+      </c>
+      <c r="K88" t="s">
+        <v>248</v>
       </c>
       <c r="L88" t="s">
         <v>66</v>
@@ -4167,25 +4167,37 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="B89" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="C89" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="D89" t="s">
         <v>249</v>
       </c>
       <c r="E89" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F89" t="s">
-        <v>395</v>
-      </c>
-      <c r="L89" t="s">
-        <v>66</v>
+        <v>404</v>
+      </c>
+      <c r="G89" t="s">
+        <v>248</v>
+      </c>
+      <c r="H89" t="s">
+        <v>248</v>
+      </c>
+      <c r="I89" t="s">
+        <v>248</v>
+      </c>
+      <c r="J89" t="s">
+        <v>248</v>
+      </c>
+      <c r="K89" t="s">
+        <v>248</v>
       </c>
       <c r="M89" t="s">
         <v>64</v>
@@ -4193,7 +4205,7 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B90" t="s">
         <v>204</v>
@@ -4208,13 +4220,13 @@
         <v>62</v>
       </c>
       <c r="F90" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="L90" t="s">
         <v>66</v>
       </c>
       <c r="M90" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="N90" t="s">
         <v>65</v>
@@ -4222,7 +4234,7 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="B91" t="s">
         <v>204</v>
@@ -4237,13 +4249,13 @@
         <v>62</v>
       </c>
       <c r="F91" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="L91" t="s">
         <v>66</v>
       </c>
       <c r="M91" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="N91" t="s">
         <v>65</v>
@@ -4251,7 +4263,7 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>402</v>
+        <v>454</v>
       </c>
       <c r="B92" t="s">
         <v>204</v>
@@ -4266,15 +4278,128 @@
         <v>62</v>
       </c>
       <c r="F92" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="L92" t="s">
         <v>66</v>
       </c>
       <c r="M92" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="N92" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>393</v>
+      </c>
+      <c r="B93" t="s">
+        <v>204</v>
+      </c>
+      <c r="C93" t="s">
+        <v>399</v>
+      </c>
+      <c r="D93" t="s">
+        <v>249</v>
+      </c>
+      <c r="E93" t="s">
+        <v>62</v>
+      </c>
+      <c r="F93" t="s">
+        <v>395</v>
+      </c>
+      <c r="L93" t="s">
+        <v>66</v>
+      </c>
+      <c r="M93" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>394</v>
+      </c>
+      <c r="B94" t="s">
+        <v>204</v>
+      </c>
+      <c r="C94" t="s">
+        <v>399</v>
+      </c>
+      <c r="D94" t="s">
+        <v>249</v>
+      </c>
+      <c r="E94" t="s">
+        <v>62</v>
+      </c>
+      <c r="F94" t="s">
+        <v>396</v>
+      </c>
+      <c r="L94" t="s">
+        <v>66</v>
+      </c>
+      <c r="M94" t="s">
+        <v>197</v>
+      </c>
+      <c r="N94" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>400</v>
+      </c>
+      <c r="B95" t="s">
+        <v>204</v>
+      </c>
+      <c r="C95" t="s">
+        <v>399</v>
+      </c>
+      <c r="D95" t="s">
+        <v>249</v>
+      </c>
+      <c r="E95" t="s">
+        <v>62</v>
+      </c>
+      <c r="F95" t="s">
+        <v>401</v>
+      </c>
+      <c r="L95" t="s">
+        <v>66</v>
+      </c>
+      <c r="M95" t="s">
+        <v>197</v>
+      </c>
+      <c r="N95" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>402</v>
+      </c>
+      <c r="B96" t="s">
+        <v>204</v>
+      </c>
+      <c r="C96" t="s">
+        <v>399</v>
+      </c>
+      <c r="D96" t="s">
+        <v>249</v>
+      </c>
+      <c r="E96" t="s">
+        <v>62</v>
+      </c>
+      <c r="F96" t="s">
+        <v>403</v>
+      </c>
+      <c r="L96" t="s">
+        <v>66</v>
+      </c>
+      <c r="M96" t="s">
+        <v>197</v>
+      </c>
+      <c r="N96" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6695,13 +6820,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C65" t="s">
         <v>429</v>
-      </c>
-      <c r="C65" t="s">
-        <v>433</v>
       </c>
       <c r="D65">
         <v>900</v>
@@ -6709,13 +6834,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C66" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D66">
         <v>901</v>
@@ -6723,13 +6848,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C67" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D67">
         <v>902</v>
@@ -6737,13 +6862,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C68" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D68">
         <v>950</v>

</xml_diff>

<commit_message>
allow for checkbox tree generation on add step
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\ErythronDBWebsite\Model\lib\wdk\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{82C47B4A-4BAC-428E-A7D4-C6D9F1D0B1D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3306506D-36A1-4CEC-9972-0F42503FC847}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="6" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="472">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1278,24 +1278,12 @@
     <t>exp_technique</t>
   </si>
   <si>
-    <t>DatasetRecordClasses.DatasetRecordClass.primary_contact</t>
-  </si>
-  <si>
     <t>primary_contact</t>
   </si>
   <si>
-    <t>DatasetRecordClasses.DatasetRecordClass.primary_publication</t>
-  </si>
-  <si>
     <t>primary_publication</t>
   </si>
   <si>
-    <t>DatasetRecordClasses.DatasetRecordClass.bulk_download_url</t>
-  </si>
-  <si>
-    <t>DatasetRecordClasses.DatasetRecordClass.organism</t>
-  </si>
-  <si>
     <t>bulk_download_url</t>
   </si>
   <si>
@@ -1308,15 +1296,9 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>DatasetRecordClasses.DatasetRecordClass.full_description</t>
-  </si>
-  <si>
     <t>full_description</t>
   </si>
   <si>
-    <t>DatasetRecordClasses.DatasetRecordClass.data_type</t>
-  </si>
-  <si>
     <t>data_type</t>
   </si>
   <si>
@@ -1464,9 +1446,6 @@
     <t>study005_questions.study005_expression</t>
   </si>
   <si>
-    <t>DatasetRecordClasses.DatasetRecordClass.primary_publication_pubmed_url</t>
-  </si>
-  <si>
     <t>study001_gene_profiles</t>
   </si>
   <si>
@@ -1531,6 +1510,21 @@
   </si>
   <si>
     <t>record_taxon</t>
+  </si>
+  <si>
+    <t>study_access</t>
+  </si>
+  <si>
+    <t>http://www.cbil.upenn.edu/ErythronDB/study003_q</t>
+  </si>
+  <si>
+    <t>http://www.cbil.upenn.edu/ErythronDB/study001_q</t>
+  </si>
+  <si>
+    <t>http://www.cbil.upenn.edu/ErythronDB/study002_q</t>
+  </si>
+  <si>
+    <t>http://www.cbil.upenn.edu/ErythronDB/study005_q</t>
   </si>
 </sst>
 </file>
@@ -1575,10 +1569,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1872,13 +1867,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N101" sqref="N101"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2020,16 +2015,22 @@
         <v>156</v>
       </c>
       <c r="D10" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="L10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" t="s">
         <v>27</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2044,16 +2045,22 @@
         <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="L11" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" t="s">
         <v>27</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2068,16 +2075,22 @@
         <v>156</v>
       </c>
       <c r="D12" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
         <v>27</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2092,16 +2105,22 @@
         <v>156</v>
       </c>
       <c r="D13" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="L13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" t="s">
         <v>27</v>
+      </c>
+      <c r="N13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2116,16 +2135,22 @@
         <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="L14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" t="s">
         <v>27</v>
+      </c>
+      <c r="N14" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2140,16 +2165,22 @@
         <v>156</v>
       </c>
       <c r="D15" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="L15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" t="s">
         <v>27</v>
+      </c>
+      <c r="N15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2157,23 +2188,29 @@
         <f>CONCATENATE(D16,".",F16)</f>
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_questions.study003_comparison</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>424</v>
+      <c r="B16" s="3" t="s">
+        <v>468</v>
       </c>
       <c r="C16" t="s">
+        <v>423</v>
+      </c>
+      <c r="D16" t="s">
         <v>429</v>
-      </c>
-      <c r="D16" t="s">
-        <v>435</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="L16" t="s">
+        <v>66</v>
+      </c>
+      <c r="M16" t="s">
         <v>27</v>
+      </c>
+      <c r="N16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2181,26 +2218,32 @@
         <f t="shared" si="0"/>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_comparison</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>422</v>
+      <c r="B17" s="3" t="s">
+        <v>469</v>
       </c>
       <c r="C17" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D17" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17" t="s">
         <v>27</v>
+      </c>
+      <c r="N17" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -2208,26 +2251,32 @@
         <f t="shared" si="0"/>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_expression</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>422</v>
+      <c r="B18" s="3" t="s">
+        <v>469</v>
       </c>
       <c r="C18" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D18" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="K18">
         <v>2</v>
       </c>
       <c r="L18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" t="s">
         <v>27</v>
+      </c>
+      <c r="N18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -2235,26 +2284,32 @@
         <f t="shared" si="0"/>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_comparison</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>423</v>
+      <c r="B19" s="3" t="s">
+        <v>470</v>
       </c>
       <c r="C19" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D19" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="K19">
         <v>3</v>
       </c>
       <c r="L19" t="s">
+        <v>66</v>
+      </c>
+      <c r="M19" t="s">
         <v>27</v>
+      </c>
+      <c r="N19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -2262,26 +2317,32 @@
         <f t="shared" si="0"/>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_expression</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>423</v>
+      <c r="B20" s="3" t="s">
+        <v>470</v>
       </c>
       <c r="C20" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D20" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="K20">
         <v>4</v>
       </c>
       <c r="L20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" t="s">
         <v>27</v>
+      </c>
+      <c r="N20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -2289,26 +2350,32 @@
         <f t="shared" si="0"/>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_comparison</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>428</v>
+      <c r="B21" s="3" t="s">
+        <v>471</v>
       </c>
       <c r="C21" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D21" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="K21">
         <v>5</v>
       </c>
       <c r="L21" t="s">
+        <v>66</v>
+      </c>
+      <c r="M21" t="s">
         <v>27</v>
+      </c>
+      <c r="N21" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -2316,31 +2383,37 @@
         <f>CONCATENATE(D22,".",F22)</f>
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_expression</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>428</v>
+      <c r="B22" s="3" t="s">
+        <v>471</v>
       </c>
       <c r="C22" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D22" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="K22">
         <v>6</v>
       </c>
       <c r="L22" t="s">
+        <v>66</v>
+      </c>
+      <c r="M22" t="s">
         <v>27</v>
+      </c>
+      <c r="N22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2355,7 +2428,7 @@
         <v>156</v>
       </c>
       <c r="D26" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E26" t="s">
         <v>62</v>
@@ -2385,13 +2458,13 @@
         <v>156</v>
       </c>
       <c r="D27" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E27" t="s">
         <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="J27" t="s">
         <v>193</v>
@@ -2421,7 +2494,7 @@
         <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E28" t="s">
         <v>62</v>
@@ -2457,7 +2530,7 @@
         <v>156</v>
       </c>
       <c r="D29" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E29" t="s">
         <v>62</v>
@@ -2493,7 +2566,7 @@
         <v>156</v>
       </c>
       <c r="D30" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E30" t="s">
         <v>62</v>
@@ -2529,7 +2602,7 @@
         <v>156</v>
       </c>
       <c r="D31" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E31" t="s">
         <v>62</v>
@@ -2565,7 +2638,7 @@
         <v>156</v>
       </c>
       <c r="D32" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E32" t="s">
         <v>62</v>
@@ -2598,13 +2671,13 @@
         <v>156</v>
       </c>
       <c r="D33" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E33" t="s">
         <v>62</v>
       </c>
       <c r="F33" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="J33" t="s">
         <v>193</v>
@@ -2628,13 +2701,13 @@
         <v>156</v>
       </c>
       <c r="D34" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E34" t="s">
         <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="J34" t="s">
         <v>193</v>
@@ -2658,13 +2731,13 @@
         <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E35" t="s">
         <v>62</v>
       </c>
       <c r="F35" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="J35" t="s">
         <v>193</v>
@@ -2694,13 +2767,13 @@
         <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E36" t="s">
         <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="J36" t="s">
         <v>193</v>
@@ -2730,7 +2803,7 @@
         <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E37" t="s">
         <v>62</v>
@@ -2763,13 +2836,13 @@
         <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E38" t="s">
         <v>62</v>
       </c>
       <c r="F38" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="J38" t="s">
         <v>193</v>
@@ -2796,7 +2869,7 @@
         <v>175</v>
       </c>
       <c r="D39" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E39" t="s">
         <v>62</v>
@@ -2829,7 +2902,7 @@
         <v>175</v>
       </c>
       <c r="D40" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E40" t="s">
         <v>62</v>
@@ -2862,13 +2935,13 @@
         <v>159</v>
       </c>
       <c r="D41" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E41" t="s">
         <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J41" t="s">
         <v>193</v>
@@ -2892,13 +2965,13 @@
         <v>159</v>
       </c>
       <c r="D42" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E42" t="s">
         <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="J42" t="s">
         <v>193</v>
@@ -2922,13 +2995,13 @@
         <v>159</v>
       </c>
       <c r="D43" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E43" t="s">
         <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="J43" t="s">
         <v>193</v>
@@ -2952,13 +3025,13 @@
         <v>159</v>
       </c>
       <c r="D44" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E44" t="s">
         <v>85</v>
       </c>
       <c r="F44" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="J44" t="s">
         <v>193</v>
@@ -2982,13 +3055,13 @@
         <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E45" t="s">
         <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="J45" t="s">
         <v>193</v>
@@ -3012,13 +3085,13 @@
         <v>173</v>
       </c>
       <c r="D46" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E46" t="s">
         <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="J46" t="s">
         <v>193</v>
@@ -3036,19 +3109,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_within_lineage_comparisons</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C47" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D47" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E47" t="s">
         <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="J47" t="s">
         <v>193</v>
@@ -3069,19 +3142,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_across_lineage_comparisons</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C48" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D48" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E48" t="s">
         <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="J48" t="s">
         <v>193</v>
@@ -3102,19 +3175,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_reporter_profiles</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C49" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D49" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E49" t="s">
         <v>85</v>
       </c>
       <c r="F49" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="J49" t="s">
         <v>193</v>
@@ -3132,19 +3205,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_gene_profiles</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C50" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D50" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E50" t="s">
         <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="J50" t="s">
         <v>193</v>
@@ -3162,19 +3235,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_lineage_comparisons</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C51" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D51" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E51" t="s">
         <v>85</v>
       </c>
       <c r="F51" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="J51" t="s">
         <v>193</v>
@@ -3195,19 +3268,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_treatment_comparisons</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C52" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D52" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E52" t="s">
         <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="J52" t="s">
         <v>193</v>
@@ -3228,19 +3301,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_reporter_profiles</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C53" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D53" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E53" t="s">
         <v>85</v>
       </c>
       <c r="F53" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="J53" t="s">
         <v>193</v>
@@ -3258,19 +3331,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_gene_profiles</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C54" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D54" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E54" t="s">
         <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="J54" t="s">
         <v>193</v>
@@ -3288,19 +3361,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_genotype_comparisons</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C55" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D55" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E55" t="s">
         <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="J55" t="s">
         <v>193</v>
@@ -3321,19 +3394,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_treatment_comparisons</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C56" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D56" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E56" t="s">
         <v>85</v>
       </c>
       <c r="F56" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="J56" t="s">
         <v>193</v>
@@ -3354,19 +3427,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_reporter_profiles</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C57" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D57" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E57" t="s">
         <v>85</v>
       </c>
       <c r="F57" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="J57" t="s">
         <v>193</v>
@@ -3384,19 +3457,19 @@
         <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_gene_profiles</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C58" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D58" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E58" t="s">
         <v>85</v>
       </c>
       <c r="F58" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="J58" t="s">
         <v>193</v>
@@ -3410,7 +3483,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -3425,7 +3498,7 @@
         <v>156</v>
       </c>
       <c r="D62" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E62" t="s">
         <v>62</v>
@@ -3455,13 +3528,13 @@
         <v>156</v>
       </c>
       <c r="D63" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E63" t="s">
         <v>62</v>
       </c>
       <c r="F63" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="J63" t="s">
         <v>193</v>
@@ -3491,7 +3564,7 @@
         <v>156</v>
       </c>
       <c r="D64" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E64" t="s">
         <v>62</v>
@@ -3527,7 +3600,7 @@
         <v>156</v>
       </c>
       <c r="D65" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E65" t="s">
         <v>62</v>
@@ -3563,7 +3636,7 @@
         <v>156</v>
       </c>
       <c r="D66" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E66" t="s">
         <v>62</v>
@@ -3599,7 +3672,7 @@
         <v>156</v>
       </c>
       <c r="D67" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E67" t="s">
         <v>62</v>
@@ -3635,7 +3708,7 @@
         <v>156</v>
       </c>
       <c r="D68" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E68" t="s">
         <v>62</v>
@@ -3668,13 +3741,13 @@
         <v>156</v>
       </c>
       <c r="D69" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E69" t="s">
         <v>62</v>
       </c>
       <c r="F69" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="J69" t="s">
         <v>193</v>
@@ -3698,13 +3771,13 @@
         <v>156</v>
       </c>
       <c r="D70" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E70" t="s">
         <v>62</v>
       </c>
       <c r="F70" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="J70" t="s">
         <v>193</v>
@@ -3728,13 +3801,13 @@
         <v>162</v>
       </c>
       <c r="D71" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E71" t="s">
         <v>62</v>
       </c>
       <c r="F71" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="J71" t="s">
         <v>193</v>
@@ -3764,13 +3837,13 @@
         <v>162</v>
       </c>
       <c r="D72" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E72" t="s">
         <v>62</v>
       </c>
       <c r="F72" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="J72" t="s">
         <v>193</v>
@@ -3800,7 +3873,7 @@
         <v>162</v>
       </c>
       <c r="D73" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E73" t="s">
         <v>62</v>
@@ -3833,13 +3906,13 @@
         <v>162</v>
       </c>
       <c r="D74" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E74" t="s">
         <v>62</v>
       </c>
       <c r="F74" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="J74" t="s">
         <v>193</v>
@@ -3866,7 +3939,7 @@
         <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E75" t="s">
         <v>62</v>
@@ -3899,7 +3972,7 @@
         <v>175</v>
       </c>
       <c r="D76" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E76" t="s">
         <v>62</v>
@@ -3932,13 +4005,13 @@
         <v>159</v>
       </c>
       <c r="D77" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E77" t="s">
         <v>85</v>
       </c>
       <c r="F77" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J77" t="s">
         <v>193</v>
@@ -3962,13 +4035,13 @@
         <v>159</v>
       </c>
       <c r="D78" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E78" t="s">
         <v>85</v>
       </c>
       <c r="F78" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="J78" t="s">
         <v>193</v>
@@ -3992,13 +4065,13 @@
         <v>159</v>
       </c>
       <c r="D79" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E79" t="s">
         <v>85</v>
       </c>
       <c r="F79" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="J79" t="s">
         <v>193</v>
@@ -4022,13 +4095,13 @@
         <v>159</v>
       </c>
       <c r="D80" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E80" t="s">
         <v>85</v>
       </c>
       <c r="F80" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="J80" t="s">
         <v>193</v>
@@ -4052,13 +4125,13 @@
         <v>173</v>
       </c>
       <c r="D81" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E81" t="s">
         <v>85</v>
       </c>
       <c r="F81" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="J81" t="s">
         <v>193</v>
@@ -4082,13 +4155,13 @@
         <v>173</v>
       </c>
       <c r="D82" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E82" t="s">
         <v>85</v>
       </c>
       <c r="F82" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="J82" t="s">
         <v>193</v>
@@ -4106,19 +4179,19 @@
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_ptm</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C83" t="s">
+        <v>423</v>
+      </c>
+      <c r="D83" t="s">
         <v>429</v>
-      </c>
-      <c r="D83" t="s">
-        <v>435</v>
       </c>
       <c r="E83" t="s">
         <v>85</v>
       </c>
       <c r="F83" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="J83" t="s">
         <v>193</v>
@@ -4139,19 +4212,19 @@
         <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_comparisons</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C84" t="s">
+        <v>423</v>
+      </c>
+      <c r="D84" t="s">
         <v>429</v>
-      </c>
-      <c r="D84" t="s">
-        <v>435</v>
       </c>
       <c r="E84" t="s">
         <v>85</v>
       </c>
       <c r="F84" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="J84" t="s">
         <v>193</v>
@@ -4180,7 +4253,7 @@
         <v>204</v>
       </c>
       <c r="C88" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D88" t="s">
         <v>249</v>
@@ -4189,7 +4262,7 @@
         <v>62</v>
       </c>
       <c r="F88" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="G88" t="s">
         <v>248</v>
@@ -4212,14 +4285,14 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
-        <f>CONCATENATE(D89,".",F89)</f>
+        <f t="shared" ref="A89:A102" si="16">CONCATENATE(D89,".",F89)</f>
         <v>DatasetRecordClasses.DatasetRecordClass.search_comparison</v>
       </c>
       <c r="B89" t="s">
         <v>204</v>
       </c>
       <c r="C89" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D89" t="s">
         <v>249</v>
@@ -4228,7 +4301,7 @@
         <v>62</v>
       </c>
       <c r="F89" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="G89" t="s">
         <v>248</v>
@@ -4250,14 +4323,15 @@
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>389</v>
+      <c r="A90" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.primary_contact</v>
       </c>
       <c r="B90" t="s">
         <v>204</v>
       </c>
       <c r="C90" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D90" t="s">
         <v>249</v>
@@ -4266,7 +4340,7 @@
         <v>62</v>
       </c>
       <c r="F90" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L90" t="s">
         <v>66</v>
@@ -4279,14 +4353,15 @@
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>391</v>
+      <c r="A91" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.primary_publication</v>
       </c>
       <c r="B91" t="s">
         <v>204</v>
       </c>
       <c r="C91" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D91" t="s">
         <v>249</v>
@@ -4295,7 +4370,7 @@
         <v>62</v>
       </c>
       <c r="F91" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L91" t="s">
         <v>66</v>
@@ -4308,14 +4383,15 @@
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>394</v>
+      <c r="A92" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.organism</v>
       </c>
       <c r="B92" t="s">
         <v>204</v>
       </c>
       <c r="C92" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D92" t="s">
         <v>249</v>
@@ -4324,7 +4400,7 @@
         <v>62</v>
       </c>
       <c r="F92" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="L92" t="s">
         <v>66</v>
@@ -4337,14 +4413,15 @@
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>399</v>
+      <c r="A93" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.full_description</v>
       </c>
       <c r="B93" t="s">
         <v>204</v>
       </c>
       <c r="C93" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D93" t="s">
         <v>249</v>
@@ -4353,7 +4430,7 @@
         <v>62</v>
       </c>
       <c r="F93" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="L93" t="s">
         <v>66</v>
@@ -4366,14 +4443,15 @@
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>401</v>
+      <c r="A94" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.data_type</v>
       </c>
       <c r="B94" t="s">
         <v>204</v>
       </c>
       <c r="C94" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D94" t="s">
         <v>249</v>
@@ -4382,7 +4460,7 @@
         <v>62</v>
       </c>
       <c r="F94" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="L94" t="s">
         <v>66</v>
@@ -4396,14 +4474,14 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
-        <f t="shared" ref="A95:A96" si="16">CONCATENATE(D95,".",F95)</f>
+        <f t="shared" si="16"/>
         <v>DatasetRecordClasses.DatasetRecordClass.protocol_images</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C95" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="D95" t="s">
         <v>249</v>
@@ -4412,7 +4490,7 @@
         <v>85</v>
       </c>
       <c r="F95" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="K95">
         <v>2</v>
@@ -4427,10 +4505,10 @@
         <v>DatasetRecordClasses.DatasetRecordClass.protocol_description</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C96" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="D96" t="s">
         <v>249</v>
@@ -4439,7 +4517,7 @@
         <v>62</v>
       </c>
       <c r="F96" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="K96">
         <v>1</v>
@@ -4449,14 +4527,15 @@
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>451</v>
+      <c r="A97" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.primary_publication</v>
       </c>
       <c r="B97" t="s">
         <v>204</v>
       </c>
       <c r="C97" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D97" t="s">
         <v>249</v>
@@ -4465,7 +4544,7 @@
         <v>62</v>
       </c>
       <c r="F97" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L97" t="s">
         <v>66</v>
@@ -4479,14 +4558,14 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
-        <f>CONCATENATE(D98,".",F98)</f>
+        <f t="shared" si="16"/>
         <v>DatasetRecordClasses.DatasetRecordClass.microarray_datasets</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C98" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D98" t="s">
         <v>249</v>
@@ -4495,7 +4574,7 @@
         <v>62</v>
       </c>
       <c r="F98" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="M98" t="s">
         <v>197</v>
@@ -4503,14 +4582,14 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
-        <f>CONCATENATE(D99,".",F99)</f>
+        <f t="shared" si="16"/>
         <v>DatasetRecordClasses.DatasetRecordClass.proteomics_datasets</v>
       </c>
       <c r="B99" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C99" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="D99" t="s">
         <v>249</v>
@@ -4519,18 +4598,19 @@
         <v>62</v>
       </c>
       <c r="F99" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>393</v>
+      <c r="A100" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.bulk_download_url</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C100" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D100" t="s">
         <v>249</v>
@@ -4539,21 +4619,22 @@
         <v>62</v>
       </c>
       <c r="F100" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="M100" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>389</v>
+      <c r="A101" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.record_taxon</v>
       </c>
       <c r="B101" t="s">
         <v>204</v>
       </c>
       <c r="C101" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D101" t="s">
         <v>249</v>
@@ -4562,10 +4643,31 @@
         <v>62</v>
       </c>
       <c r="F101" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="M101" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102" t="str">
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.study_access</v>
+      </c>
+      <c r="B102" t="s">
+        <v>204</v>
+      </c>
+      <c r="C102" t="s">
+        <v>394</v>
+      </c>
+      <c r="D102" t="s">
+        <v>249</v>
+      </c>
+      <c r="E102" t="s">
+        <v>62</v>
+      </c>
+      <c r="F102" t="s">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -4574,6 +4676,13 @@
     <hyperlink ref="B95" r:id="rId2" location="http://edamontology.org/topic_3934" display="https://ifb-elixirfr.github.io/edam-browser/ - http://edamontology.org/topic_3934" xr:uid="{D64BE6B9-0C24-4330-9E69-59D2AFAB68FD}"/>
     <hyperlink ref="B98" r:id="rId3" xr:uid="{E33DF20E-8197-497E-ACBC-9A7D8C6B61E9}"/>
     <hyperlink ref="B100" r:id="rId4" xr:uid="{7BEA3C84-8210-4D98-BC03-B17F03A7A315}"/>
+    <hyperlink ref="B16" r:id="rId5" xr:uid="{77374C50-9DA7-4029-86EA-90D1EAEB2CD8}"/>
+    <hyperlink ref="B17" r:id="rId6" xr:uid="{6A8B9933-A376-4B67-AEA0-F78BE733288C}"/>
+    <hyperlink ref="B18" r:id="rId7" xr:uid="{134E537B-1ED0-44E3-9238-5DBC0B83B820}"/>
+    <hyperlink ref="B19" r:id="rId8" xr:uid="{8BB624E1-F50C-404E-9011-F65592F215C3}"/>
+    <hyperlink ref="B20" r:id="rId9" xr:uid="{A52DFD08-1FC0-4210-9576-DDDC1C0DE9B9}"/>
+    <hyperlink ref="B21" r:id="rId10" xr:uid="{DFA1871A-B92C-4090-A7A3-04AC5E96B789}"/>
+    <hyperlink ref="B22" r:id="rId11" xr:uid="{11978A85-F4C4-4280-AD6C-AEEF995C1E86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6213,7 +6322,7 @@
         <v>204</v>
       </c>
       <c r="C9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -6465,7 +6574,7 @@
         <v>217</v>
       </c>
       <c r="C27" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D27">
         <v>27</v>
@@ -6991,13 +7100,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C65" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D65">
         <v>900</v>
@@ -7005,13 +7114,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C66" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D66">
         <v>901</v>
@@ -7019,13 +7128,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C67" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D67">
         <v>902</v>
@@ -7033,13 +7142,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C68" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="D68">
         <v>950</v>
@@ -7047,13 +7156,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C69" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="D69">
         <v>50</v>
@@ -7061,13 +7170,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="C70" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D70">
         <v>55</v>
@@ -7075,13 +7184,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C71" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="D71">
         <v>52</v>
@@ -7089,13 +7198,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="B72" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C72" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="D72">
         <v>53</v>

</xml_diff>

<commit_message>
add questions for filtering / enrichment results / documentation fixes
</commit_message>
<xml_diff>
--- a/Model/lib/wdk/ontology/individuals.xlsx
+++ b/Model/lib/wdk/ontology/individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\wsl_share\ErythronDBWebsite\Model\lib\wdk\ontology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74F5095-58A5-455B-99D8-31FD2C03822C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0AD7F796-4173-413A-BBB6-DCC96B308AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34260" yWindow="5670" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="commonIndividuals" localSheetId="3">common!$A$1:$N$36</definedName>
-    <definedName name="individuals" localSheetId="0">individuals!$A$1:$N$63</definedName>
+    <definedName name="individuals" localSheetId="0">individuals!$A$1:$N$61</definedName>
     <definedName name="individuals" localSheetId="1">orthomcl!$A$1:$N$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="471">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1407,24 +1407,6 @@
     <t>study003_comparisons</t>
   </si>
   <si>
-    <t>MouseGeneQuestions.go</t>
-  </si>
-  <si>
-    <t>HumanGeneQuestions.go</t>
-  </si>
-  <si>
-    <t>MouseGeneQuestions.upload</t>
-  </si>
-  <si>
-    <t>HumanGeneQuestions.upload</t>
-  </si>
-  <si>
-    <t>MouseGeneQuestions.pathways</t>
-  </si>
-  <si>
-    <t>HumanGeneQuestions.pathways</t>
-  </si>
-  <si>
     <t>study003_questions.study003_comparison</t>
   </si>
   <si>
@@ -1528,6 +1510,18 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>hs_questions.hs_gene_keyword</t>
+  </si>
+  <si>
+    <t>mm_questions.mm_gene_keyword</t>
+  </si>
+  <si>
+    <t>mm_questions.mm_upload</t>
+  </si>
+  <si>
+    <t>hs_questions.hs_upload</t>
   </si>
 </sst>
 </file>
@@ -1870,13 +1864,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B57DF8-3481-BA45-B7D4-B0110941E0EF}">
-  <dimension ref="A1:N103"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L59" sqref="L59"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2009,13 +2003,13 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE(D10,".",F10)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.HumanGeneQuestions.upload</v>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.hs_questions.hs_upload</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>429</v>
@@ -2024,7 +2018,10 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>435</v>
+        <v>470</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
       </c>
       <c r="L10" t="s">
         <v>66</v>
@@ -2038,14 +2035,14 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" ref="A11:A21" si="0">CONCATENATE(D11,".",F11)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.MouseGeneQuestions.upload</v>
+        <f t="shared" ref="A11:A19" si="0">CONCATENATE(D11,".",F11)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.mm_questions.mm_upload</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>407</v>
@@ -2054,7 +2051,10 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>434</v>
+        <v>469</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
       </c>
       <c r="L11" t="s">
         <v>66</v>
@@ -2068,14 +2068,14 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.MouseGeneQuestions.go</v>
+        <f>CONCATENATE(D12,".",F12)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.mm_questions.mm_gene_keyword</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>407</v>
@@ -2084,7 +2084,10 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>432</v>
+        <v>468</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
       </c>
       <c r="L12" t="s">
         <v>66</v>
@@ -2098,14 +2101,14 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" ref="A13:A14" si="1">CONCATENATE(D13,".",F13)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.HumanGeneQuestions.go</v>
+        <f t="shared" ref="A13" si="1">CONCATENATE(D13,".",F13)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.hs_questions.hs_gene_keyword</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>429</v>
@@ -2114,7 +2117,10 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>433</v>
+        <v>467</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
       </c>
       <c r="L13" t="s">
         <v>66</v>
@@ -2128,23 +2134,23 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" si="1"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.MouseGeneQuestions.pathways</v>
-      </c>
-      <c r="B14" t="s">
-        <v>155</v>
+        <f>CONCATENATE(D14,".",F14)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_questions.study003_comparison</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>462</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>423</v>
       </c>
       <c r="D14" t="s">
-        <v>407</v>
+        <v>429</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="L14" t="s">
         <v>66</v>
@@ -2158,23 +2164,26 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" ref="A15" si="2">CONCATENATE(D15,".",F15)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.HumanGeneQuestions.pathways</v>
-      </c>
-      <c r="B15" t="s">
-        <v>155</v>
+        <f t="shared" si="0"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_comparison</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>463</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>420</v>
       </c>
       <c r="D15" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>437</v>
+        <v>433</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
       </c>
       <c r="L15" t="s">
         <v>66</v>
@@ -2188,23 +2197,26 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>CONCATENATE(D16,".",F16)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_questions.study003_comparison</v>
+        <f t="shared" si="0"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_expression</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C16" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D16" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>438</v>
+        <v>434</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
       </c>
       <c r="L16" t="s">
         <v>66</v>
@@ -2219,13 +2231,13 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_comparison</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_comparison</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D17" t="s">
         <v>407</v>
@@ -2234,10 +2246,10 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L17" t="s">
         <v>66</v>
@@ -2252,13 +2264,13 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_questions.study001_expression</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_expression</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D18" t="s">
         <v>407</v>
@@ -2267,10 +2279,10 @@
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="K18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L18" t="s">
         <v>66</v>
@@ -2285,13 +2297,13 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_comparison</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_comparison</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="C19" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="D19" t="s">
         <v>407</v>
@@ -2300,10 +2312,10 @@
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L19" t="s">
         <v>66</v>
@@ -2317,14 +2329,14 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_questions.study002_expression</v>
+        <f>CONCATENATE(D20,".",F20)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_expression</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="C20" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="D20" t="s">
         <v>407</v>
@@ -2333,10 +2345,10 @@
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="K20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L20" t="s">
         <v>66</v>
@@ -2348,81 +2360,81 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <f t="shared" si="0"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_comparison</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="C21" t="s">
-        <v>424</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>CONCATENATE(D24,".",F24)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.source_id</v>
+      </c>
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" t="s">
         <v>407</v>
       </c>
-      <c r="E21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" t="s">
-        <v>443</v>
-      </c>
-      <c r="K21">
-        <v>5</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" t="s">
+        <v>193</v>
+      </c>
+      <c r="M24" t="s">
+        <v>197</v>
+      </c>
+      <c r="N24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" ref="A25:A45" si="2">CONCATENATE(D25,".",F25)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.organism</v>
+      </c>
+      <c r="B25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" t="s">
+        <v>407</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" t="s">
+        <v>392</v>
+      </c>
+      <c r="J25" t="s">
+        <v>193</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
         <v>66</v>
       </c>
-      <c r="M21" t="s">
-        <v>27</v>
-      </c>
-      <c r="N21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <f>CONCATENATE(D22,".",F22)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_questions.study005_expression</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="C22" t="s">
-        <v>424</v>
-      </c>
-      <c r="D22" t="s">
-        <v>407</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" t="s">
-        <v>444</v>
-      </c>
-      <c r="K22">
-        <v>6</v>
-      </c>
-      <c r="L22" t="s">
-        <v>66</v>
-      </c>
-      <c r="M22" t="s">
-        <v>27</v>
-      </c>
-      <c r="N22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>397</v>
+      <c r="M25" t="s">
+        <v>197</v>
+      </c>
+      <c r="N25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>CONCATENATE(D26,".",F26)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.source_id</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.symbol</v>
       </c>
       <c r="B26" t="s">
         <v>155</v>
@@ -2437,11 +2449,17 @@
         <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>127</v>
+        <v>243</v>
       </c>
       <c r="J26" t="s">
         <v>193</v>
       </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26" t="s">
+        <v>66</v>
+      </c>
       <c r="M26" t="s">
         <v>197</v>
       </c>
@@ -2451,8 +2469,8 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" ref="A27:A47" si="3">CONCATENATE(D27,".",F27)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.organism</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.product</v>
       </c>
       <c r="B27" t="s">
         <v>155</v>
@@ -2467,13 +2485,13 @@
         <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>392</v>
+        <v>131</v>
       </c>
       <c r="J27" t="s">
         <v>193</v>
       </c>
       <c r="K27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L27" t="s">
         <v>66</v>
@@ -2488,7 +2506,7 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>CONCATENATE(D28,".",F28)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.symbol</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.synonym</v>
       </c>
       <c r="B28" t="s">
         <v>155</v>
@@ -2503,13 +2521,13 @@
         <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J28" t="s">
         <v>193</v>
       </c>
       <c r="K28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L28" t="s">
         <v>66</v>
@@ -2523,8 +2541,8 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.product</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.gene_type</v>
       </c>
       <c r="B29" t="s">
         <v>155</v>
@@ -2539,13 +2557,13 @@
         <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>131</v>
+        <v>209</v>
       </c>
       <c r="J29" t="s">
         <v>193</v>
       </c>
       <c r="K29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L29" t="s">
         <v>66</v>
@@ -2560,7 +2578,7 @@
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>CONCATENATE(D30,".",F30)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.synonym</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_record_link</v>
       </c>
       <c r="B30" t="s">
         <v>155</v>
@@ -2575,13 +2593,13 @@
         <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J30" t="s">
         <v>193</v>
       </c>
       <c r="K30">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L30" t="s">
         <v>66</v>
@@ -2589,14 +2607,11 @@
       <c r="M30" t="s">
         <v>197</v>
       </c>
-      <c r="N30" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.gene_type</v>
+        <f t="shared" ref="A31:A32" si="3">CONCATENATE(D31,".",F31)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_source_id</v>
       </c>
       <c r="B31" t="s">
         <v>155</v>
@@ -2611,19 +2626,13 @@
         <v>62</v>
       </c>
       <c r="F31" t="s">
-        <v>209</v>
+        <v>411</v>
       </c>
       <c r="J31" t="s">
         <v>193</v>
       </c>
       <c r="K31">
-        <v>5</v>
-      </c>
-      <c r="L31" t="s">
-        <v>66</v>
-      </c>
-      <c r="M31" t="s">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="N31" t="s">
         <v>65</v>
@@ -2631,8 +2640,8 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>CONCATENATE(D32,".",F32)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_record_link</v>
+        <f t="shared" si="3"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_symbol</v>
       </c>
       <c r="B32" t="s">
         <v>155</v>
@@ -2647,7 +2656,7 @@
         <v>62</v>
       </c>
       <c r="F32" t="s">
-        <v>242</v>
+        <v>412</v>
       </c>
       <c r="J32" t="s">
         <v>193</v>
@@ -2655,23 +2664,20 @@
       <c r="K32">
         <v>6</v>
       </c>
-      <c r="L32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M32" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" ref="A33:A34" si="4">CONCATENATE(D33,".",F33)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_source_id</v>
+        <f>CONCATENATE(D33,".",F33)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.locus</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
         <v>407</v>
@@ -2680,13 +2686,19 @@
         <v>62</v>
       </c>
       <c r="F33" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J33" t="s">
         <v>193</v>
       </c>
       <c r="K33">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>66</v>
+      </c>
+      <c r="M33" t="s">
+        <v>197</v>
       </c>
       <c r="N33" t="s">
         <v>65</v>
@@ -2694,14 +2706,14 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="4"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.ortholog_symbol</v>
+        <f>CONCATENATE(D34,".",F34)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.location</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D34" t="s">
         <v>407</v>
@@ -2710,22 +2722,28 @@
         <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="J34" t="s">
         <v>193</v>
       </c>
       <c r="K34">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="L34" t="s">
+        <v>66</v>
+      </c>
+      <c r="M34" t="s">
+        <v>197</v>
       </c>
       <c r="N34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>CONCATENATE(D35,".",F35)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.locus</v>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.chromosome</v>
       </c>
       <c r="B35" t="s">
         <v>162</v>
@@ -2740,14 +2758,11 @@
         <v>62</v>
       </c>
       <c r="F35" t="s">
-        <v>409</v>
+        <v>208</v>
       </c>
       <c r="J35" t="s">
         <v>193</v>
       </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
       <c r="L35" t="s">
         <v>66</v>
       </c>
@@ -2760,8 +2775,8 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>CONCATENATE(D36,".",F36)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.location</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.strand</v>
       </c>
       <c r="B36" t="s">
         <v>162</v>
@@ -2776,14 +2791,11 @@
         <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J36" t="s">
         <v>193</v>
       </c>
-      <c r="K36">
-        <v>2</v>
-      </c>
       <c r="L36" t="s">
         <v>66</v>
       </c>
@@ -2796,14 +2808,14 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>CONCATENATE(D37,".",F37)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.chromosome</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.start_min</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="D37" t="s">
         <v>407</v>
@@ -2812,7 +2824,7 @@
         <v>62</v>
       </c>
       <c r="F37" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J37" t="s">
         <v>193</v>
@@ -2829,14 +2841,14 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.strand</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.end_max</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="D38" t="s">
         <v>407</v>
@@ -2845,7 +2857,7 @@
         <v>62</v>
       </c>
       <c r="F38" t="s">
-        <v>408</v>
+        <v>207</v>
       </c>
       <c r="J38" t="s">
         <v>193</v>
@@ -2862,32 +2874,29 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.start_min</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.gene_link_outs</v>
       </c>
       <c r="B39" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C39" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D39" t="s">
         <v>407</v>
       </c>
       <c r="E39" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F39" t="s">
-        <v>206</v>
+        <v>399</v>
       </c>
       <c r="J39" t="s">
         <v>193</v>
       </c>
-      <c r="L39" t="s">
-        <v>66</v>
-      </c>
       <c r="M39" t="s">
-        <v>197</v>
+        <v>64</v>
       </c>
       <c r="N39" t="s">
         <v>65</v>
@@ -2895,32 +2904,29 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.end_max</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.protein_link_outs</v>
       </c>
       <c r="B40" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C40" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D40" t="s">
         <v>407</v>
       </c>
       <c r="E40" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F40" t="s">
-        <v>207</v>
+        <v>400</v>
       </c>
       <c r="J40" t="s">
         <v>193</v>
       </c>
-      <c r="L40" t="s">
-        <v>66</v>
-      </c>
       <c r="M40" t="s">
-        <v>197</v>
+        <v>64</v>
       </c>
       <c r="N40" t="s">
         <v>65</v>
@@ -2928,8 +2934,8 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.gene_link_outs</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.clinical_link_outs</v>
       </c>
       <c r="B41" t="s">
         <v>157</v>
@@ -2944,7 +2950,7 @@
         <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="J41" t="s">
         <v>193</v>
@@ -2958,8 +2964,8 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.protein_link_outs</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.sequence_link_outs</v>
       </c>
       <c r="B42" t="s">
         <v>157</v>
@@ -2974,7 +2980,7 @@
         <v>85</v>
       </c>
       <c r="F42" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="J42" t="s">
         <v>193</v>
@@ -2988,14 +2994,14 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.clinical_link_outs</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.pathways</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D43" t="s">
         <v>407</v>
@@ -3004,7 +3010,7 @@
         <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="J43" t="s">
         <v>193</v>
@@ -3018,14 +3024,14 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.sequence_link_outs</v>
+        <f t="shared" ref="A44" si="4">CONCATENATE(D44,".",F44)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.go_terms</v>
       </c>
       <c r="B44" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C44" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
         <v>407</v>
@@ -3034,7 +3040,7 @@
         <v>85</v>
       </c>
       <c r="F44" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J44" t="s">
         <v>193</v>
@@ -3048,14 +3054,14 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.pathways</v>
-      </c>
-      <c r="B45" t="s">
-        <v>172</v>
+        <f t="shared" si="2"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_within_lineage_comparisons</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>416</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>420</v>
       </c>
       <c r="D45" t="s">
         <v>407</v>
@@ -3064,11 +3070,14 @@
         <v>85</v>
       </c>
       <c r="F45" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="J45" t="s">
         <v>193</v>
       </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
       <c r="M45" t="s">
         <v>64</v>
       </c>
@@ -3078,14 +3087,14 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" ref="A46" si="5">CONCATENATE(D46,".",F46)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.go_terms</v>
-      </c>
-      <c r="B46" t="s">
-        <v>172</v>
+        <f t="shared" ref="A46:A49" si="5">CONCATENATE(D46,".",F46)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_across_lineage_comparisons</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>416</v>
       </c>
       <c r="C46" t="s">
-        <v>173</v>
+        <v>420</v>
       </c>
       <c r="D46" t="s">
         <v>407</v>
@@ -3094,11 +3103,14 @@
         <v>85</v>
       </c>
       <c r="F46" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="J46" t="s">
         <v>193</v>
       </c>
+      <c r="K46">
+        <v>4</v>
+      </c>
       <c r="M46" t="s">
         <v>64</v>
       </c>
@@ -3108,8 +3120,8 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="3"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_within_lineage_comparisons</v>
+        <f>CONCATENATE(D47,".",F47)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_reporter_profiles</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>416</v>
@@ -3124,25 +3136,22 @@
         <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>405</v>
+        <v>440</v>
       </c>
       <c r="J47" t="s">
         <v>193</v>
       </c>
       <c r="K47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M47" t="s">
         <v>64</v>
       </c>
-      <c r="N47" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" ref="A48:A51" si="6">CONCATENATE(D48,".",F48)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_across_lineage_comparisons</v>
+        <f t="shared" si="5"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_gene_profiles</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>416</v>
@@ -3157,31 +3166,28 @@
         <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>406</v>
+        <v>439</v>
       </c>
       <c r="J48" t="s">
         <v>193</v>
       </c>
       <c r="K48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M48" t="s">
         <v>64</v>
       </c>
-      <c r="N48" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>CONCATENATE(D49,".",F49)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_reporter_profiles</v>
+        <f t="shared" si="5"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_lineage_comparisons</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C49" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D49" t="s">
         <v>407</v>
@@ -3190,28 +3196,31 @@
         <v>85</v>
       </c>
       <c r="F49" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="J49" t="s">
         <v>193</v>
       </c>
       <c r="K49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M49" t="s">
         <v>64</v>
       </c>
+      <c r="N49" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" si="6"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study001_gene_profiles</v>
+        <f t="shared" ref="A50" si="6">CONCATENATE(D50,".",F50)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_treatment_comparisons</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C50" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D50" t="s">
         <v>407</v>
@@ -3220,22 +3229,25 @@
         <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>445</v>
+        <v>426</v>
       </c>
       <c r="J50" t="s">
         <v>193</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M50" t="s">
         <v>64</v>
       </c>
+      <c r="N50" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f t="shared" si="6"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_lineage_comparisons</v>
+        <f t="shared" ref="A51:A55" si="7">CONCATENATE(D51,".",F51)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_reporter_profiles</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>417</v>
@@ -3250,25 +3262,22 @@
         <v>85</v>
       </c>
       <c r="F51" t="s">
-        <v>425</v>
+        <v>443</v>
       </c>
       <c r="J51" t="s">
         <v>193</v>
       </c>
       <c r="K51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M51" t="s">
         <v>64</v>
       </c>
-      <c r="N51" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f t="shared" ref="A52" si="7">CONCATENATE(D52,".",F52)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_treatment_comparisons</v>
+        <f t="shared" ref="A52" si="8">CONCATENATE(D52,".",F52)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_gene_profiles</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>417</v>
@@ -3283,31 +3292,28 @@
         <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>426</v>
+        <v>444</v>
       </c>
       <c r="J52" t="s">
         <v>193</v>
       </c>
       <c r="K52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M52" t="s">
         <v>64</v>
       </c>
-      <c r="N52" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" ref="A53:A57" si="8">CONCATENATE(D53,".",F53)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_reporter_profiles</v>
+        <f t="shared" si="7"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_genotype_comparisons</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="C53" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="D53" t="s">
         <v>407</v>
@@ -3316,28 +3322,31 @@
         <v>85</v>
       </c>
       <c r="F53" t="s">
-        <v>449</v>
+        <v>427</v>
       </c>
       <c r="J53" t="s">
         <v>193</v>
       </c>
       <c r="K53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M53" t="s">
         <v>64</v>
       </c>
+      <c r="N53" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f t="shared" ref="A54" si="9">CONCATENATE(D54,".",F54)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study002_gene_profiles</v>
+        <f>CONCATENATE(D54,".",F54)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_treatment_comparisons</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="C54" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="D54" t="s">
         <v>407</v>
@@ -3346,22 +3355,25 @@
         <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>450</v>
+        <v>428</v>
       </c>
       <c r="J54" t="s">
         <v>193</v>
       </c>
       <c r="K54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M54" t="s">
         <v>64</v>
       </c>
+      <c r="N54" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f t="shared" si="8"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_genotype_comparisons</v>
+        <f t="shared" si="7"/>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_reporter_profiles</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>422</v>
@@ -3376,25 +3388,22 @@
         <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>427</v>
+        <v>441</v>
       </c>
       <c r="J55" t="s">
         <v>193</v>
       </c>
       <c r="K55">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M55" t="s">
         <v>64</v>
       </c>
-      <c r="N55" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>CONCATENATE(D56,".",F56)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_treatment_comparisons</v>
+        <f t="shared" ref="A56" si="9">CONCATENATE(D56,".",F56)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_gene_profiles</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>422</v>
@@ -3409,123 +3418,126 @@
         <v>85</v>
       </c>
       <c r="F56" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="J56" t="s">
         <v>193</v>
       </c>
       <c r="K56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M56" t="s">
         <v>64</v>
       </c>
-      <c r="N56" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f t="shared" si="8"/>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_reporter_profiles</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>422</v>
+        <f t="shared" ref="A57" si="10">CONCATENATE(D57,".",F57)</f>
+        <v>MouseGeneRecordClasses.MouseGeneRecordClass.note</v>
+      </c>
+      <c r="B57" t="s">
+        <v>155</v>
       </c>
       <c r="C57" t="s">
-        <v>424</v>
+        <v>156</v>
       </c>
       <c r="D57" t="s">
         <v>407</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="F57" t="s">
-        <v>447</v>
+        <v>466</v>
       </c>
       <c r="J57" t="s">
         <v>193</v>
       </c>
       <c r="K57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M57" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" t="str">
-        <f t="shared" ref="A58" si="10">CONCATENATE(D58,".",F58)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.study005_gene_profiles</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C58" t="s">
-        <v>424</v>
-      </c>
-      <c r="D58" t="s">
-        <v>407</v>
-      </c>
-      <c r="E58" t="s">
-        <v>85</v>
-      </c>
-      <c r="F58" t="s">
-        <v>448</v>
-      </c>
-      <c r="J58" t="s">
+        <v>197</v>
+      </c>
+      <c r="N57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f t="shared" ref="A61:A62" si="11">CONCATENATE(D61,".",F61)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.source_id</v>
+      </c>
+      <c r="B61" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" t="s">
+        <v>429</v>
+      </c>
+      <c r="E61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F61" t="s">
+        <v>127</v>
+      </c>
+      <c r="J61" t="s">
         <v>193</v>
       </c>
-      <c r="K58">
+      <c r="M61" t="s">
+        <v>197</v>
+      </c>
+      <c r="N61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
+        <f t="shared" si="11"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.organism</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" t="s">
+        <v>156</v>
+      </c>
+      <c r="D62" t="s">
+        <v>429</v>
+      </c>
+      <c r="E62" t="s">
+        <v>62</v>
+      </c>
+      <c r="F62" t="s">
+        <v>392</v>
+      </c>
+      <c r="J62" t="s">
+        <v>193</v>
+      </c>
+      <c r="K62">
         <v>1</v>
       </c>
-      <c r="M58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
-        <f t="shared" ref="A59" si="11">CONCATENATE(D59,".",F59)</f>
-        <v>MouseGeneRecordClasses.MouseGeneRecordClass.note</v>
-      </c>
-      <c r="B59" t="s">
-        <v>155</v>
-      </c>
-      <c r="C59" t="s">
-        <v>156</v>
-      </c>
-      <c r="D59" t="s">
-        <v>407</v>
-      </c>
-      <c r="E59" t="s">
-        <v>62</v>
-      </c>
-      <c r="F59" t="s">
-        <v>472</v>
-      </c>
-      <c r="J59" t="s">
-        <v>193</v>
-      </c>
-      <c r="K59">
-        <v>1</v>
-      </c>
-      <c r="M59" t="s">
+      <c r="L62" t="s">
+        <v>66</v>
+      </c>
+      <c r="M62" t="s">
         <v>197</v>
       </c>
-      <c r="N59" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>398</v>
+      <c r="N62" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f t="shared" ref="A63:A64" si="12">CONCATENATE(D63,".",F63)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.source_id</v>
+        <f>CONCATENATE(D63,".",F63)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.symbol</v>
       </c>
       <c r="B63" t="s">
         <v>155</v>
@@ -3540,11 +3552,17 @@
         <v>62</v>
       </c>
       <c r="F63" t="s">
-        <v>127</v>
+        <v>243</v>
       </c>
       <c r="J63" t="s">
         <v>193</v>
       </c>
+      <c r="K63">
+        <v>2</v>
+      </c>
+      <c r="L63" t="s">
+        <v>66</v>
+      </c>
       <c r="M63" t="s">
         <v>197</v>
       </c>
@@ -3554,8 +3572,8 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f t="shared" si="12"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.organism</v>
+        <f t="shared" ref="A64" si="12">CONCATENATE(D64,".",F64)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.product</v>
       </c>
       <c r="B64" t="s">
         <v>155</v>
@@ -3570,13 +3588,13 @@
         <v>62</v>
       </c>
       <c r="F64" t="s">
-        <v>392</v>
+        <v>131</v>
       </c>
       <c r="J64" t="s">
         <v>193</v>
       </c>
       <c r="K64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L64" t="s">
         <v>66</v>
@@ -3591,7 +3609,7 @@
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>CONCATENATE(D65,".",F65)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.symbol</v>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.synonym</v>
       </c>
       <c r="B65" t="s">
         <v>155</v>
@@ -3606,13 +3624,13 @@
         <v>62</v>
       </c>
       <c r="F65" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J65" t="s">
         <v>193</v>
       </c>
       <c r="K65">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L65" t="s">
         <v>66</v>
@@ -3627,7 +3645,7 @@
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" ref="A66" si="13">CONCATENATE(D66,".",F66)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.product</v>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_type</v>
       </c>
       <c r="B66" t="s">
         <v>155</v>
@@ -3642,13 +3660,13 @@
         <v>62</v>
       </c>
       <c r="F66" t="s">
-        <v>131</v>
+        <v>209</v>
       </c>
       <c r="J66" t="s">
         <v>193</v>
       </c>
       <c r="K66">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L66" t="s">
         <v>66</v>
@@ -3663,7 +3681,7 @@
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>CONCATENATE(D67,".",F67)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.synonym</v>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_record_link</v>
       </c>
       <c r="B67" t="s">
         <v>155</v>
@@ -3678,13 +3696,13 @@
         <v>62</v>
       </c>
       <c r="F67" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J67" t="s">
         <v>193</v>
       </c>
       <c r="K67">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L67" t="s">
         <v>66</v>
@@ -3692,14 +3710,11 @@
       <c r="M67" t="s">
         <v>197</v>
       </c>
-      <c r="N67" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f t="shared" ref="A68" si="14">CONCATENATE(D68,".",F68)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_type</v>
+        <f t="shared" ref="A68:A69" si="14">CONCATENATE(D68,".",F68)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_source_id</v>
       </c>
       <c r="B68" t="s">
         <v>155</v>
@@ -3714,19 +3729,13 @@
         <v>62</v>
       </c>
       <c r="F68" t="s">
-        <v>209</v>
+        <v>411</v>
       </c>
       <c r="J68" t="s">
         <v>193</v>
       </c>
       <c r="K68">
-        <v>5</v>
-      </c>
-      <c r="L68" t="s">
-        <v>66</v>
-      </c>
-      <c r="M68" t="s">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="N68" t="s">
         <v>65</v>
@@ -3734,8 +3743,8 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f>CONCATENATE(D69,".",F69)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_record_link</v>
+        <f t="shared" si="14"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_symbol</v>
       </c>
       <c r="B69" t="s">
         <v>155</v>
@@ -3750,7 +3759,7 @@
         <v>62</v>
       </c>
       <c r="F69" t="s">
-        <v>242</v>
+        <v>412</v>
       </c>
       <c r="J69" t="s">
         <v>193</v>
@@ -3758,23 +3767,20 @@
       <c r="K69">
         <v>6</v>
       </c>
-      <c r="L69" t="s">
-        <v>66</v>
-      </c>
-      <c r="M69" t="s">
-        <v>197</v>
+      <c r="N69" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f t="shared" ref="A70:A71" si="15">CONCATENATE(D70,".",F70)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_source_id</v>
+        <f>CONCATENATE(D70,".",F70)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.locus</v>
       </c>
       <c r="B70" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D70" t="s">
         <v>429</v>
@@ -3783,13 +3789,19 @@
         <v>62</v>
       </c>
       <c r="F70" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J70" t="s">
         <v>193</v>
       </c>
       <c r="K70">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="L70" t="s">
+        <v>66</v>
+      </c>
+      <c r="M70" t="s">
+        <v>197</v>
       </c>
       <c r="N70" t="s">
         <v>65</v>
@@ -3797,14 +3809,14 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f t="shared" si="15"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.ortholog_symbol</v>
+        <f>CONCATENATE(D71,".",F71)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.location</v>
       </c>
       <c r="B71" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C71" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D71" t="s">
         <v>429</v>
@@ -3813,13 +3825,19 @@
         <v>62</v>
       </c>
       <c r="F71" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="J71" t="s">
         <v>193</v>
       </c>
       <c r="K71">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="L71" t="s">
+        <v>66</v>
+      </c>
+      <c r="M71" t="s">
+        <v>197</v>
       </c>
       <c r="N71" t="s">
         <v>65</v>
@@ -3828,7 +3846,7 @@
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>CONCATENATE(D72,".",F72)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.locus</v>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.chromosome</v>
       </c>
       <c r="B72" t="s">
         <v>162</v>
@@ -3843,14 +3861,11 @@
         <v>62</v>
       </c>
       <c r="F72" t="s">
-        <v>409</v>
+        <v>208</v>
       </c>
       <c r="J72" t="s">
         <v>193</v>
       </c>
-      <c r="K72">
-        <v>1</v>
-      </c>
       <c r="L72" t="s">
         <v>66</v>
       </c>
@@ -3863,8 +3878,8 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f>CONCATENATE(D73,".",F73)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.location</v>
+        <f t="shared" ref="A73:A83" si="15">CONCATENATE(D73,".",F73)</f>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.strand</v>
       </c>
       <c r="B73" t="s">
         <v>162</v>
@@ -3879,14 +3894,11 @@
         <v>62</v>
       </c>
       <c r="F73" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J73" t="s">
         <v>193</v>
       </c>
-      <c r="K73">
-        <v>2</v>
-      </c>
       <c r="L73" t="s">
         <v>66</v>
       </c>
@@ -3899,14 +3911,14 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f>CONCATENATE(D74,".",F74)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.chromosome</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.start_min</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C74" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="D74" t="s">
         <v>429</v>
@@ -3915,7 +3927,7 @@
         <v>62</v>
       </c>
       <c r="F74" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J74" t="s">
         <v>193</v>
@@ -3932,14 +3944,14 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f t="shared" ref="A75:A85" si="16">CONCATENATE(D75,".",F75)</f>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.strand</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.end_max</v>
       </c>
       <c r="B75" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C75" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="D75" t="s">
         <v>429</v>
@@ -3948,7 +3960,7 @@
         <v>62</v>
       </c>
       <c r="F75" t="s">
-        <v>408</v>
+        <v>207</v>
       </c>
       <c r="J75" t="s">
         <v>193</v>
@@ -3965,32 +3977,29 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.start_min</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_link_outs</v>
       </c>
       <c r="B76" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C76" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D76" t="s">
         <v>429</v>
       </c>
       <c r="E76" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F76" t="s">
-        <v>206</v>
+        <v>399</v>
       </c>
       <c r="J76" t="s">
         <v>193</v>
       </c>
-      <c r="L76" t="s">
-        <v>66</v>
-      </c>
       <c r="M76" t="s">
-        <v>197</v>
+        <v>64</v>
       </c>
       <c r="N76" t="s">
         <v>65</v>
@@ -3998,32 +4007,29 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.end_max</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.protein_link_outs</v>
       </c>
       <c r="B77" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C77" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D77" t="s">
         <v>429</v>
       </c>
       <c r="E77" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F77" t="s">
-        <v>207</v>
+        <v>400</v>
       </c>
       <c r="J77" t="s">
         <v>193</v>
       </c>
-      <c r="L77" t="s">
-        <v>66</v>
-      </c>
       <c r="M77" t="s">
-        <v>197</v>
+        <v>64</v>
       </c>
       <c r="N77" t="s">
         <v>65</v>
@@ -4031,8 +4037,8 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.gene_link_outs</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.clinical_link_outs</v>
       </c>
       <c r="B78" t="s">
         <v>157</v>
@@ -4047,7 +4053,7 @@
         <v>85</v>
       </c>
       <c r="F78" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="J78" t="s">
         <v>193</v>
@@ -4061,8 +4067,8 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.protein_link_outs</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.sequence_link_outs</v>
       </c>
       <c r="B79" t="s">
         <v>157</v>
@@ -4077,7 +4083,7 @@
         <v>85</v>
       </c>
       <c r="F79" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="J79" t="s">
         <v>193</v>
@@ -4091,14 +4097,14 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.clinical_link_outs</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.pathways</v>
       </c>
       <c r="B80" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D80" t="s">
         <v>429</v>
@@ -4107,7 +4113,7 @@
         <v>85</v>
       </c>
       <c r="F80" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="J80" t="s">
         <v>193</v>
@@ -4121,14 +4127,14 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.sequence_link_outs</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.go_terms</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C81" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D81" t="s">
         <v>429</v>
@@ -4137,7 +4143,7 @@
         <v>85</v>
       </c>
       <c r="F81" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J81" t="s">
         <v>193</v>
@@ -4151,14 +4157,14 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.pathways</v>
-      </c>
-      <c r="B82" t="s">
-        <v>172</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_ptm</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>418</v>
       </c>
       <c r="C82" t="s">
-        <v>173</v>
+        <v>423</v>
       </c>
       <c r="D82" t="s">
         <v>429</v>
@@ -4167,11 +4173,14 @@
         <v>85</v>
       </c>
       <c r="F82" t="s">
-        <v>404</v>
+        <v>430</v>
       </c>
       <c r="J82" t="s">
         <v>193</v>
       </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
       <c r="M82" t="s">
         <v>64</v>
       </c>
@@ -4181,14 +4190,14 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.go_terms</v>
-      </c>
-      <c r="B83" t="s">
-        <v>172</v>
+        <f t="shared" si="15"/>
+        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_comparisons</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>418</v>
       </c>
       <c r="C83" t="s">
-        <v>173</v>
+        <v>423</v>
       </c>
       <c r="D83" t="s">
         <v>429</v>
@@ -4197,11 +4206,14 @@
         <v>85</v>
       </c>
       <c r="F83" t="s">
-        <v>403</v>
+        <v>431</v>
       </c>
       <c r="J83" t="s">
         <v>193</v>
       </c>
+      <c r="K83">
+        <v>2</v>
+      </c>
       <c r="M83" t="s">
         <v>64</v>
       </c>
@@ -4209,81 +4221,93 @@
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_ptm</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C84" t="s">
-        <v>423</v>
-      </c>
-      <c r="D84" t="s">
-        <v>429</v>
-      </c>
-      <c r="E84" t="s">
-        <v>85</v>
-      </c>
-      <c r="F84" t="s">
-        <v>430</v>
-      </c>
-      <c r="J84" t="s">
-        <v>193</v>
-      </c>
-      <c r="K84">
-        <v>1</v>
-      </c>
-      <c r="M84" t="s">
-        <v>64</v>
-      </c>
-      <c r="N84" t="s">
-        <v>65</v>
-      </c>
-    </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" t="str">
-        <f t="shared" si="16"/>
-        <v>HumanGeneRecordClasses.HumanGeneRecordClass.study003_comparisons</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C85" t="s">
-        <v>423</v>
-      </c>
-      <c r="D85" t="s">
-        <v>429</v>
-      </c>
-      <c r="E85" t="s">
-        <v>85</v>
-      </c>
-      <c r="F85" t="s">
-        <v>431</v>
-      </c>
-      <c r="J85" t="s">
-        <v>193</v>
-      </c>
-      <c r="K85">
-        <v>2</v>
-      </c>
-      <c r="M85" t="s">
-        <v>64</v>
-      </c>
-      <c r="N85" t="s">
-        <v>65</v>
+      <c r="A85" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>247</v>
+      <c r="A87" t="str">
+        <f>CONCATENATE(D87,".",F87)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.search_expression</v>
+      </c>
+      <c r="B87" t="s">
+        <v>204</v>
+      </c>
+      <c r="C87" t="s">
+        <v>394</v>
+      </c>
+      <c r="D87" t="s">
+        <v>249</v>
+      </c>
+      <c r="E87" t="s">
+        <v>62</v>
+      </c>
+      <c r="F87" t="s">
+        <v>446</v>
+      </c>
+      <c r="G87" t="s">
+        <v>248</v>
+      </c>
+      <c r="H87" t="s">
+        <v>248</v>
+      </c>
+      <c r="I87" t="s">
+        <v>248</v>
+      </c>
+      <c r="J87" t="s">
+        <v>248</v>
+      </c>
+      <c r="K87" t="s">
+        <v>248</v>
+      </c>
+      <c r="M87" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
+        <f t="shared" ref="A88:A101" si="16">CONCATENATE(D88,".",F88)</f>
+        <v>DatasetRecordClasses.DatasetRecordClass.search_comparison</v>
+      </c>
+      <c r="B88" t="s">
+        <v>204</v>
+      </c>
+      <c r="C88" t="s">
+        <v>394</v>
+      </c>
+      <c r="D88" t="s">
+        <v>249</v>
+      </c>
+      <c r="E88" t="s">
+        <v>62</v>
+      </c>
+      <c r="F88" t="s">
+        <v>459</v>
+      </c>
+      <c r="G88" t="s">
+        <v>248</v>
+      </c>
+      <c r="H88" t="s">
+        <v>248</v>
+      </c>
+      <c r="I88" t="s">
+        <v>248</v>
+      </c>
+      <c r="J88" t="s">
+        <v>248</v>
+      </c>
+      <c r="K88" t="s">
+        <v>248</v>
+      </c>
+      <c r="M88" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
-        <f>CONCATENATE(D89,".",F89)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.search_expression</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.primary_contact</v>
       </c>
       <c r="B89" t="s">
         <v>204</v>
@@ -4298,31 +4322,22 @@
         <v>62</v>
       </c>
       <c r="F89" t="s">
-        <v>452</v>
-      </c>
-      <c r="G89" t="s">
-        <v>248</v>
-      </c>
-      <c r="H89" t="s">
-        <v>248</v>
-      </c>
-      <c r="I89" t="s">
-        <v>248</v>
-      </c>
-      <c r="J89" t="s">
-        <v>248</v>
-      </c>
-      <c r="K89" t="s">
-        <v>248</v>
+        <v>389</v>
+      </c>
+      <c r="L89" t="s">
+        <v>66</v>
       </c>
       <c r="M89" t="s">
         <v>197</v>
       </c>
+      <c r="N89" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
-        <f t="shared" ref="A90:A103" si="17">CONCATENATE(D90,".",F90)</f>
-        <v>DatasetRecordClasses.DatasetRecordClass.search_comparison</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.primary_publication</v>
       </c>
       <c r="B90" t="s">
         <v>204</v>
@@ -4337,31 +4352,22 @@
         <v>62</v>
       </c>
       <c r="F90" t="s">
-        <v>465</v>
-      </c>
-      <c r="G90" t="s">
-        <v>248</v>
-      </c>
-      <c r="H90" t="s">
-        <v>248</v>
-      </c>
-      <c r="I90" t="s">
-        <v>248</v>
-      </c>
-      <c r="J90" t="s">
-        <v>248</v>
-      </c>
-      <c r="K90" t="s">
-        <v>248</v>
+        <v>390</v>
+      </c>
+      <c r="L90" t="s">
+        <v>66</v>
       </c>
       <c r="M90" t="s">
         <v>197</v>
       </c>
+      <c r="N90" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.primary_contact</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.organism</v>
       </c>
       <c r="B91" t="s">
         <v>204</v>
@@ -4376,7 +4382,7 @@
         <v>62</v>
       </c>
       <c r="F91" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="L91" t="s">
         <v>66</v>
@@ -4390,8 +4396,8 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.primary_publication</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.full_description</v>
       </c>
       <c r="B92" t="s">
         <v>204</v>
@@ -4406,7 +4412,7 @@
         <v>62</v>
       </c>
       <c r="F92" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="L92" t="s">
         <v>66</v>
@@ -4420,8 +4426,8 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.organism</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.data_type</v>
       </c>
       <c r="B93" t="s">
         <v>204</v>
@@ -4436,7 +4442,7 @@
         <v>62</v>
       </c>
       <c r="F93" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="L93" t="s">
         <v>66</v>
@@ -4450,44 +4456,41 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.full_description</v>
-      </c>
-      <c r="B94" t="s">
-        <v>204</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.protocol_images</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>448</v>
       </c>
       <c r="C94" t="s">
-        <v>394</v>
+        <v>449</v>
       </c>
       <c r="D94" t="s">
         <v>249</v>
       </c>
       <c r="E94" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="F94" t="s">
-        <v>395</v>
-      </c>
-      <c r="L94" t="s">
-        <v>66</v>
+        <v>445</v>
+      </c>
+      <c r="K94">
+        <v>2</v>
       </c>
       <c r="M94" t="s">
-        <v>197</v>
-      </c>
-      <c r="N94" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.data_type</v>
-      </c>
-      <c r="B95" t="s">
-        <v>204</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.protocol_description</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>448</v>
       </c>
       <c r="C95" t="s">
-        <v>394</v>
+        <v>449</v>
       </c>
       <c r="D95" t="s">
         <v>249</v>
@@ -4496,55 +4499,55 @@
         <v>62</v>
       </c>
       <c r="F95" t="s">
-        <v>396</v>
-      </c>
-      <c r="L95" t="s">
-        <v>66</v>
+        <v>447</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
       </c>
       <c r="M95" t="s">
-        <v>197</v>
-      </c>
-      <c r="N95" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.protocol_images</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>454</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.primary_publication</v>
+      </c>
+      <c r="B96" t="s">
+        <v>204</v>
       </c>
       <c r="C96" t="s">
-        <v>455</v>
+        <v>394</v>
       </c>
       <c r="D96" t="s">
         <v>249</v>
       </c>
       <c r="E96" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="F96" t="s">
-        <v>451</v>
-      </c>
-      <c r="K96">
-        <v>2</v>
+        <v>390</v>
+      </c>
+      <c r="L96" t="s">
+        <v>66</v>
       </c>
       <c r="M96" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="N96" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.protocol_description</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.microarray_datasets</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C97" t="s">
         <v>454</v>
-      </c>
-      <c r="C97" t="s">
-        <v>455</v>
       </c>
       <c r="D97" t="s">
         <v>249</v>
@@ -4553,25 +4556,22 @@
         <v>62</v>
       </c>
       <c r="F97" t="s">
-        <v>453</v>
-      </c>
-      <c r="K97">
-        <v>1</v>
+        <v>457</v>
       </c>
       <c r="M97" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.primary_publication</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.proteomics_datasets</v>
       </c>
       <c r="B98" t="s">
-        <v>204</v>
+        <v>455</v>
       </c>
       <c r="C98" t="s">
-        <v>394</v>
+        <v>456</v>
       </c>
       <c r="D98" t="s">
         <v>249</v>
@@ -4580,28 +4580,19 @@
         <v>62</v>
       </c>
       <c r="F98" t="s">
-        <v>390</v>
-      </c>
-      <c r="L98" t="s">
-        <v>66</v>
-      </c>
-      <c r="M98" t="s">
-        <v>197</v>
-      </c>
-      <c r="N98" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.microarray_datasets</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.bulk_download_url</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="C99" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D99" t="s">
         <v>249</v>
@@ -4610,22 +4601,22 @@
         <v>62</v>
       </c>
       <c r="F99" t="s">
-        <v>463</v>
+        <v>391</v>
       </c>
       <c r="M99" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.proteomics_datasets</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.record_taxon</v>
       </c>
       <c r="B100" t="s">
-        <v>461</v>
+        <v>204</v>
       </c>
       <c r="C100" t="s">
-        <v>462</v>
+        <v>394</v>
       </c>
       <c r="D100" t="s">
         <v>249</v>
@@ -4634,19 +4625,22 @@
         <v>62</v>
       </c>
       <c r="F100" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+      <c r="M100" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.bulk_download_url</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>459</v>
+        <f t="shared" si="16"/>
+        <v>DatasetRecordClasses.DatasetRecordClass.study_access</v>
+      </c>
+      <c r="B101" t="s">
+        <v>204</v>
       </c>
       <c r="C101" t="s">
-        <v>460</v>
+        <v>394</v>
       </c>
       <c r="D101" t="s">
         <v>249</v>
@@ -4655,70 +4649,22 @@
         <v>62</v>
       </c>
       <c r="F101" t="s">
-        <v>391</v>
-      </c>
-      <c r="M101" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A102" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.record_taxon</v>
-      </c>
-      <c r="B102" t="s">
-        <v>204</v>
-      </c>
-      <c r="C102" t="s">
-        <v>394</v>
-      </c>
-      <c r="D102" t="s">
-        <v>249</v>
-      </c>
-      <c r="E102" t="s">
-        <v>62</v>
-      </c>
-      <c r="F102" t="s">
-        <v>466</v>
-      </c>
-      <c r="M102" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A103" t="str">
-        <f t="shared" si="17"/>
-        <v>DatasetRecordClasses.DatasetRecordClass.study_access</v>
-      </c>
-      <c r="B103" t="s">
-        <v>204</v>
-      </c>
-      <c r="C103" t="s">
-        <v>394</v>
-      </c>
-      <c r="D103" t="s">
-        <v>249</v>
-      </c>
-      <c r="E103" t="s">
-        <v>62</v>
-      </c>
-      <c r="F103" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B97" r:id="rId1" location="http://edamontology.org/topic_3934" display="https://ifb-elixirfr.github.io/edam-browser/ - http://edamontology.org/topic_3934" xr:uid="{04B9D51A-0900-4B93-B368-0849FF381F1D}"/>
-    <hyperlink ref="B96" r:id="rId2" location="http://edamontology.org/topic_3934" display="https://ifb-elixirfr.github.io/edam-browser/ - http://edamontology.org/topic_3934" xr:uid="{D64BE6B9-0C24-4330-9E69-59D2AFAB68FD}"/>
-    <hyperlink ref="B99" r:id="rId3" xr:uid="{E33DF20E-8197-497E-ACBC-9A7D8C6B61E9}"/>
-    <hyperlink ref="B101" r:id="rId4" xr:uid="{7BEA3C84-8210-4D98-BC03-B17F03A7A315}"/>
-    <hyperlink ref="B16" r:id="rId5" xr:uid="{77374C50-9DA7-4029-86EA-90D1EAEB2CD8}"/>
-    <hyperlink ref="B17" r:id="rId6" xr:uid="{6A8B9933-A376-4B67-AEA0-F78BE733288C}"/>
-    <hyperlink ref="B18" r:id="rId7" xr:uid="{134E537B-1ED0-44E3-9238-5DBC0B83B820}"/>
-    <hyperlink ref="B19" r:id="rId8" xr:uid="{8BB624E1-F50C-404E-9011-F65592F215C3}"/>
-    <hyperlink ref="B20" r:id="rId9" xr:uid="{A52DFD08-1FC0-4210-9576-DDDC1C0DE9B9}"/>
-    <hyperlink ref="B21" r:id="rId10" xr:uid="{DFA1871A-B92C-4090-A7A3-04AC5E96B789}"/>
-    <hyperlink ref="B22" r:id="rId11" xr:uid="{11978A85-F4C4-4280-AD6C-AEEF995C1E86}"/>
+    <hyperlink ref="B95" r:id="rId1" location="http://edamontology.org/topic_3934" display="https://ifb-elixirfr.github.io/edam-browser/ - http://edamontology.org/topic_3934" xr:uid="{04B9D51A-0900-4B93-B368-0849FF381F1D}"/>
+    <hyperlink ref="B94" r:id="rId2" location="http://edamontology.org/topic_3934" display="https://ifb-elixirfr.github.io/edam-browser/ - http://edamontology.org/topic_3934" xr:uid="{D64BE6B9-0C24-4330-9E69-59D2AFAB68FD}"/>
+    <hyperlink ref="B97" r:id="rId3" xr:uid="{E33DF20E-8197-497E-ACBC-9A7D8C6B61E9}"/>
+    <hyperlink ref="B99" r:id="rId4" xr:uid="{7BEA3C84-8210-4D98-BC03-B17F03A7A315}"/>
+    <hyperlink ref="B14" r:id="rId5" xr:uid="{77374C50-9DA7-4029-86EA-90D1EAEB2CD8}"/>
+    <hyperlink ref="B15" r:id="rId6" xr:uid="{6A8B9933-A376-4B67-AEA0-F78BE733288C}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{134E537B-1ED0-44E3-9238-5DBC0B83B820}"/>
+    <hyperlink ref="B17" r:id="rId8" xr:uid="{8BB624E1-F50C-404E-9011-F65592F215C3}"/>
+    <hyperlink ref="B18" r:id="rId9" xr:uid="{A52DFD08-1FC0-4210-9576-DDDC1C0DE9B9}"/>
+    <hyperlink ref="B19" r:id="rId10" xr:uid="{DFA1871A-B92C-4090-A7A3-04AC5E96B789}"/>
+    <hyperlink ref="B20" r:id="rId11" xr:uid="{11978A85-F4C4-4280-AD6C-AEEF995C1E86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7192,13 +7138,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="C69" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D69">
         <v>50</v>
@@ -7206,13 +7152,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C70" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="D70">
         <v>55</v>
@@ -7220,13 +7166,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="C71" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D71">
         <v>52</v>
@@ -7234,13 +7180,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="B72" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C72" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="D72">
         <v>53</v>

</xml_diff>